<commit_message>
Sorting logic implemented when clicked on table header names
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A4AF2C-A099-484E-87CD-4365AF5DFFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DAA647-DA96-4303-A7BA-B26686B2AA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
@@ -1294,32 +1294,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1343,6 +1322,27 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1661,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20:S20"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,1426 +1672,1450 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="26"/>
     </row>
     <row r="17" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="26"/>
     </row>
     <row r="18" spans="1:19" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
     </row>
     <row r="19" spans="1:19" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="J19" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
     </row>
     <row r="20" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="15" t="s">
+      <c r="J20" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
     </row>
     <row r="21" spans="1:19" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>3</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="15" t="s">
+      <c r="J21" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
     </row>
     <row r="22" spans="1:19" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>4</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="15" t="s">
+      <c r="J22" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
     </row>
     <row r="23" spans="1:19" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="J23" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
     </row>
     <row r="24" spans="1:19" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>6</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="15" t="s">
+      <c r="J24" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
     </row>
     <row r="25" spans="1:19" ht="109.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>7</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="J25" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
     </row>
     <row r="26" spans="1:19" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>8</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="15" t="s">
+      <c r="J26" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
     </row>
     <row r="27" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>9</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="J27" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
     </row>
     <row r="28" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>10</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="15" t="s">
+      <c r="J28" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
     </row>
     <row r="29" spans="1:19" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>11</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="15" t="s">
+      <c r="J29" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="18"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="20"/>
     </row>
     <row r="30" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>12</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="15" t="s">
+      <c r="J30" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
     </row>
     <row r="31" spans="1:19" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="15" t="s">
+      <c r="J31" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="15"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
     </row>
     <row r="32" spans="1:19" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>14</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="15" t="s">
+      <c r="J32" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="15" t="s">
+      <c r="J33" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="15"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="15" t="s">
+      <c r="J34" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="15"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>17</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="15" t="s">
+      <c r="J35" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="15"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>18</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="15" t="s">
+      <c r="J36" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="15" t="s">
+      <c r="J37" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
     </row>
     <row r="38" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>20</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="15" t="s">
+      <c r="J38" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="15" t="s">
+      <c r="J39" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
-      <c r="P39" s="15"/>
-      <c r="Q39" s="15"/>
-      <c r="R39" s="15"/>
-      <c r="S39" s="15"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>22</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="15" t="s">
+      <c r="J40" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="15"/>
-      <c r="S40" s="15"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="15" t="s">
+      <c r="J41" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-      <c r="S41" s="15"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="15" t="s">
+      <c r="J42" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="15"/>
-      <c r="S42" s="15"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="15" t="s">
+      <c r="J43" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="15" t="s">
+      <c r="J44" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="15" t="s">
+      <c r="J45" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="15"/>
-      <c r="R45" s="15"/>
-      <c r="S45" s="15"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="15" t="s">
+      <c r="J46" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
-      <c r="P46" s="15"/>
-      <c r="Q46" s="15"/>
-      <c r="R46" s="15"/>
-      <c r="S46" s="15"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="15" t="s">
+      <c r="J47" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="15"/>
-      <c r="S47" s="15"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="15" t="s">
+      <c r="J48" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="15"/>
-      <c r="R48" s="15"/>
-      <c r="S48" s="15"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="23" t="s">
+      <c r="A50" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="23"/>
-      <c r="K50" s="23"/>
-      <c r="L50" s="23"/>
-      <c r="M50" s="23"/>
-      <c r="N50" s="23"/>
-      <c r="O50" s="23"/>
-      <c r="P50" s="23"/>
-      <c r="Q50" s="23"/>
-      <c r="R50" s="23"/>
-      <c r="S50" s="23"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16"/>
+      <c r="L50" s="16"/>
+      <c r="M50" s="16"/>
+      <c r="N50" s="16"/>
+      <c r="O50" s="16"/>
+      <c r="P50" s="16"/>
+      <c r="Q50" s="16"/>
+      <c r="R50" s="16"/>
+      <c r="S50" s="16"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
-      <c r="J51" s="24"/>
-      <c r="K51" s="24"/>
-      <c r="L51" s="24"/>
-      <c r="M51" s="24"/>
-      <c r="N51" s="24"/>
-      <c r="O51" s="24"/>
-      <c r="P51" s="24"/>
-      <c r="Q51" s="24"/>
-      <c r="R51" s="24"/>
-      <c r="S51" s="25"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
+      <c r="Q51" s="17"/>
+      <c r="R51" s="17"/>
+      <c r="S51" s="18"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="19"/>
-      <c r="K52" s="19"/>
-      <c r="L52" s="19"/>
-      <c r="M52" s="19"/>
-      <c r="N52" s="19"/>
-      <c r="O52" s="19"/>
-      <c r="P52" s="19"/>
-      <c r="Q52" s="19"/>
-      <c r="R52" s="19"/>
-      <c r="S52" s="20"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+      <c r="L52" s="12"/>
+      <c r="M52" s="12"/>
+      <c r="N52" s="12"/>
+      <c r="O52" s="12"/>
+      <c r="P52" s="12"/>
+      <c r="Q52" s="12"/>
+      <c r="R52" s="12"/>
+      <c r="S52" s="13"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
-      <c r="J53" s="19"/>
-      <c r="K53" s="19"/>
-      <c r="L53" s="19"/>
-      <c r="M53" s="19"/>
-      <c r="N53" s="19"/>
-      <c r="O53" s="19"/>
-      <c r="P53" s="19"/>
-      <c r="Q53" s="19"/>
-      <c r="R53" s="19"/>
-      <c r="S53" s="20"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="12"/>
+      <c r="K53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="12"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="12"/>
+      <c r="S53" s="13"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
-      <c r="J54" s="19"/>
-      <c r="K54" s="19"/>
-      <c r="L54" s="19"/>
-      <c r="M54" s="19"/>
-      <c r="N54" s="19"/>
-      <c r="O54" s="19"/>
-      <c r="P54" s="19"/>
-      <c r="Q54" s="19"/>
-      <c r="R54" s="19"/>
-      <c r="S54" s="20"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+      <c r="K54" s="12"/>
+      <c r="L54" s="12"/>
+      <c r="M54" s="12"/>
+      <c r="N54" s="12"/>
+      <c r="O54" s="12"/>
+      <c r="P54" s="12"/>
+      <c r="Q54" s="12"/>
+      <c r="R54" s="12"/>
+      <c r="S54" s="13"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19"/>
-      <c r="J55" s="19"/>
-      <c r="K55" s="19"/>
-      <c r="L55" s="19"/>
-      <c r="M55" s="19"/>
-      <c r="N55" s="19"/>
-      <c r="O55" s="19"/>
-      <c r="P55" s="19"/>
-      <c r="Q55" s="19"/>
-      <c r="R55" s="19"/>
-      <c r="S55" s="20"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
+      <c r="N55" s="12"/>
+      <c r="O55" s="12"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12"/>
+      <c r="R55" s="12"/>
+      <c r="S55" s="13"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="21"/>
-      <c r="M56" s="21"/>
-      <c r="N56" s="21"/>
-      <c r="O56" s="21"/>
-      <c r="P56" s="21"/>
-      <c r="Q56" s="21"/>
-      <c r="R56" s="21"/>
-      <c r="S56" s="22"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="14"/>
+      <c r="N56" s="14"/>
+      <c r="O56" s="14"/>
+      <c r="P56" s="14"/>
+      <c r="Q56" s="14"/>
+      <c r="R56" s="14"/>
+      <c r="S56" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B54:S54"/>
-    <mergeCell ref="B55:S55"/>
-    <mergeCell ref="B56:S56"/>
-    <mergeCell ref="J48:S48"/>
-    <mergeCell ref="A50:S50"/>
-    <mergeCell ref="B51:S51"/>
-    <mergeCell ref="B52:S52"/>
-    <mergeCell ref="B53:S53"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="J47:S47"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="J22:S22"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="J18:S18"/>
+    <mergeCell ref="J19:S19"/>
+    <mergeCell ref="J20:S20"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J24:S24"/>
+    <mergeCell ref="J25:S25"/>
+    <mergeCell ref="J26:S26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J27:S27"/>
+    <mergeCell ref="J28:S28"/>
+    <mergeCell ref="J29:S29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="J30:S30"/>
+    <mergeCell ref="J31:S31"/>
+    <mergeCell ref="J32:S32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="J34:S34"/>
+    <mergeCell ref="J35:S35"/>
     <mergeCell ref="J45:S45"/>
     <mergeCell ref="J46:S46"/>
     <mergeCell ref="B45:H45"/>
@@ -3108,48 +3132,24 @@
     <mergeCell ref="J42:S42"/>
     <mergeCell ref="J43:S43"/>
     <mergeCell ref="J44:S44"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="J34:S34"/>
-    <mergeCell ref="J35:S35"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="J30:S30"/>
-    <mergeCell ref="J31:S31"/>
-    <mergeCell ref="J32:S32"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J27:S27"/>
-    <mergeCell ref="J28:S28"/>
-    <mergeCell ref="J29:S29"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="J24:S24"/>
-    <mergeCell ref="J25:S25"/>
-    <mergeCell ref="J26:S26"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="J18:S18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="J20:S20"/>
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="A1:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B54:S54"/>
+    <mergeCell ref="B55:S55"/>
+    <mergeCell ref="B56:S56"/>
+    <mergeCell ref="J48:S48"/>
+    <mergeCell ref="A50:S50"/>
+    <mergeCell ref="B51:S51"/>
+    <mergeCell ref="B52:S52"/>
+    <mergeCell ref="B53:S53"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="J47:S47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3157,12 +3157,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7005DF65C69D244A0053930B4D80895" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfe4224a46d45a1569ee43293fdcdd48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a217f1db-afc0-486b-a03f-32483c6d35f7" xmlns:ns4="b3fc9c33-149f-45e5-9bdb-a4f7fe310215" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d8dd93a9b58d240e8e3304885c0c0fa" ns3:_="" ns4:_="">
     <xsd:import namespace="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
@@ -3379,6 +3373,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3389,23 +3389,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D0DA503-506E-48B5-9538-4DAB746C5D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3424,6 +3407,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916385B-7771-4B86-AC30-95BD0DD5FA1F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Application settings implemented as a class (function removed)
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DAA647-DA96-4303-A7BA-B26686B2AA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8485949-E43A-4A4D-B30D-AD752815D3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
@@ -195,8 +195,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
+    <t>Svaka funkcionalnost treba biti odabrana i implementirana na način da je barem minimalno korisna u rješavanju problematike kojom se bavi vaša aplikacija. One funkcionalnosti koje ne doprinose izvornoj namjeni aplikacije ili njenim dijelovima neće biti uvažene.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Za svaki korišteni mehanizam međusobnog zaključavanja treba opisati:
 </t>
     </r>
     <r>
@@ -210,19 +213,12 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* svrha unutar aplikacije (za što se koristi baza podataka i koja je njena uloga u projektu)
-* tip baze podataka (MS Access, MS SQL Server, MySQL, Oracle…)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
+      <t xml:space="preserve">* što (koji resurs aplikacije) se zaključava, te zašto je zaključavanje potrebno </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
 </t>
     </r>
     <r>
@@ -236,7 +232,7 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* nazive tablica i za koje od njih su podržane sve CRUD (kreiraj, čitaj, ažuriraj i briši) operacije</t>
+      <t>* što predstavlja procese A i B, te zašto proces A kreira (poziva) proces B</t>
     </r>
     <r>
       <rPr>
@@ -248,15 +244,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Napomena: baza podataka ne može obrađivati podatke koji se već obrađuju korištenjem XML, JSON ili datoteke prilagođenog formata.</t>
-    </r>
-  </si>
-  <si>
-    <t>Svaka funkcionalnost treba biti odabrana i implementirana na način da je barem minimalno korisna u rješavanju problematike kojom se bavi vaša aplikacija. One funkcionalnosti koje ne doprinose izvornoj namjeni aplikacije ili njenim dijelovima neće biti uvažene.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Za svaki korišteni mehanizam međusobnog zaključavanja treba opisati:
 </t>
     </r>
     <r>
@@ -270,7 +257,7 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">* što (koji resurs aplikacije) se zaključava, te zašto je zaključavanje potrebno </t>
+      <t>* što je povratna vrijednost procesa B</t>
     </r>
   </si>
   <si>
@@ -289,83 +276,7 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* što predstavlja procese A i B, te zašto proces A kreira (poziva) proces B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* što je povratna vrijednost procesa B</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>* što se u korisničkom sučelju ažurira iz dretve</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Za svaki od pristupa (INI i/ili Windows registar) treba opisati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">* postavke aplikacije koji se spremaju
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Napomena: ukoliko se koriste oba pristupa (INI i Windows registar), oni moraju raditi s različitim postavkama aplikacije.</t>
     </r>
   </si>
   <si>
@@ -1021,12 +932,151 @@
   <si>
     <t>Aplikacija koristi barem jednu funkciju sažimanja (npr. SHA-256), 2 boda. Ukoliko se pri sažimanju koristi fiksna (svugdje ista) "sol" moguće je dobiti 3 boda, a za korištenje promjenjive "soli" moguće je dobiti 4 boda. Promjenjiva "sol" se treba generirati korištenjem nekog pravila, pri čemu nije dopušteno spremanje "soli" u bazu podataka/datoteku i sl. Za korištenje "papra" moguće je dobiti dodatna 3 boda, pri čemu je potrebno demonstrirati provjeru ispravnog "papra" kroz cijeli niz mogućih vrijednosti za taj "papar".</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* svrha unutar aplikacije (za što se koristi baza podataka i koja je njena uloga u projektu)
+* tip baze podataka (MS Access, MS SQL Server, MySQL, Oracle…)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* nazive tablica i za koje od njih su podržane sve CRUD (kreiraj, čitaj, ažuriraj i briši) operacije</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Napomena: baza podataka ne može obrađivati podatke koji se već obrađuju korištenjem XML, JSON ili datoteke prilagođenog formata.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija komentar:
+Korištena je MS Access baza podataka. Sve funkcije koje obavljaju radnje nad MS Access bazom podataka nalaze se u access_connector.py datoteci.
+Baza podataka se koristi za pohranu i dohvat korisničkih računa za pristup aplikaciji. U aplikaciji se forma 
+nalazi u create_user_form.py. Baza podataka se također koristi za pohranu stanja skladišta/dućana, tj proizvoda koji se nalaze na stanju, te nazive skladišta/dućana i osnovne podatke o njima. 
+Postoje dvije Microsoft Access Database (.accdb)
+1. proizvodi.accdb
+Ova baza podataka se koristi za spremanje informacija o proizvodima i skladištima. Sastoji se od dvije tablice 'proizvodi' i 'skladišta'. Te dvije tablice su u relaciji pomoću ključa 'skladiste_id' tako da su u relaciji, te da svako skladište može imati više proizvoda
+2. users.accdb
+Ova baza podataka se koristi za pohranu podataka za pristup aplikaciji (username i password). Te se sastoji od tablice 'credentials'. 
+Sve tablice podržavaju CRUD operacije (proizvodi, skladista i credentials)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Za svaki od pristupa (INI i/ili Windows registar) treba opisati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* postavke aplikacije koji se spremaju
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Napomena: ukoliko se koriste oba pristupa (INI i Windows registar), oni moraju raditi s različitim postavkama aplikacije.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Matija komentar:
+INI configuration file:
+Aplikacija koristi INI datoteku, te za citanje i pisanje koristi python module 'configparser'. Funkcija koja obavlja postavku se naziva 'settings' te se nalazi u python datoteci 'app.py'.
+Koristi se za tri postavke:
+1. postavke vrste fonta
+2. postavke velicine fonta
+3. postavke pozadine forme
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1107,8 +1157,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1125,8 +1182,20 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1259,13 +1328,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1294,11 +1400,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1322,26 +1449,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1661,8 +1782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:H23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25:S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,1450 +1793,1426 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
+      <c r="A7" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="26"/>
+      <c r="A16" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
     </row>
     <row r="17" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
-      <c r="S17" s="26"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
     </row>
     <row r="18" spans="1:19" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="22" t="s">
+      <c r="J18" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
     </row>
     <row r="19" spans="1:19" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
+      <c r="J19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
     </row>
     <row r="20" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
     </row>
     <row r="21" spans="1:19" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>3</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
+      <c r="J21" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
     </row>
     <row r="22" spans="1:19" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="31">
         <v>4</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="B22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
+      <c r="J22" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
     </row>
     <row r="23" spans="1:19" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="B23" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
+      <c r="J23" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
     </row>
     <row r="24" spans="1:19" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>6</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-    </row>
-    <row r="25" spans="1:19" ht="109.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="J24" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+    </row>
+    <row r="25" spans="1:19" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27">
         <v>7</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
+      <c r="J25" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="29"/>
+      <c r="S25" s="30"/>
     </row>
     <row r="26" spans="1:19" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>8</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11"/>
-      <c r="S26" s="11"/>
+      <c r="J26" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
     </row>
     <row r="27" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>9</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
+      <c r="J27" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
     </row>
     <row r="28" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>10</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
+      <c r="B28" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="11"/>
+      <c r="J28" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
     </row>
     <row r="29" spans="1:19" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>11</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
+      <c r="B29" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="20"/>
-      <c r="R29" s="20"/>
-      <c r="S29" s="20"/>
+      <c r="J29" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
     </row>
     <row r="30" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>12</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
+      <c r="J30" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
     </row>
     <row r="31" spans="1:19" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
+      <c r="B31" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="11"/>
+      <c r="J31" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
     </row>
     <row r="32" spans="1:19" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>14</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
+      <c r="J32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
+      <c r="B33" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
+      <c r="J33" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
+      <c r="B34" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
-      <c r="S34" s="11"/>
+      <c r="J34" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>17</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="11"/>
+      <c r="J35" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>18</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
+      <c r="J36" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
+      <c r="B37" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11"/>
+      <c r="J37" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
     </row>
     <row r="38" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>20</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
-      <c r="S38" s="11"/>
+      <c r="J38" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
+      <c r="B39" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="11"/>
+      <c r="J39" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="15"/>
+      <c r="S39" s="15"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>22</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
+      <c r="J40" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
+      <c r="J41" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
+      <c r="S41" s="15"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11"/>
+      <c r="J42" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="15"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
+      <c r="B43" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
-      <c r="S43" s="11"/>
+      <c r="J43" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="15"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
-      <c r="Q44" s="11"/>
-      <c r="R44" s="11"/>
-      <c r="S44" s="11"/>
+      <c r="J44" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-      <c r="S45" s="11"/>
+      <c r="J45" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
+      <c r="S45" s="15"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="11"/>
-      <c r="S46" s="11"/>
+      <c r="J46" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+      <c r="R46" s="15"/>
+      <c r="S46" s="15"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-      <c r="S47" s="11"/>
+      <c r="J47" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="15"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="11"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-      <c r="S48" s="11"/>
+      <c r="J48" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
+      <c r="S48" s="15"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
+      <c r="A50" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
-      <c r="I50" s="16"/>
-      <c r="J50" s="16"/>
-      <c r="K50" s="16"/>
-      <c r="L50" s="16"/>
-      <c r="M50" s="16"/>
-      <c r="N50" s="16"/>
-      <c r="O50" s="16"/>
-      <c r="P50" s="16"/>
-      <c r="Q50" s="16"/>
-      <c r="R50" s="16"/>
-      <c r="S50" s="16"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="23"/>
+      <c r="K50" s="23"/>
+      <c r="L50" s="23"/>
+      <c r="M50" s="23"/>
+      <c r="N50" s="23"/>
+      <c r="O50" s="23"/>
+      <c r="P50" s="23"/>
+      <c r="Q50" s="23"/>
+      <c r="R50" s="23"/>
+      <c r="S50" s="23"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
-      <c r="J51" s="17"/>
-      <c r="K51" s="17"/>
-      <c r="L51" s="17"/>
-      <c r="M51" s="17"/>
-      <c r="N51" s="17"/>
-      <c r="O51" s="17"/>
-      <c r="P51" s="17"/>
-      <c r="Q51" s="17"/>
-      <c r="R51" s="17"/>
-      <c r="S51" s="18"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="24"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="24"/>
+      <c r="N51" s="24"/>
+      <c r="O51" s="24"/>
+      <c r="P51" s="24"/>
+      <c r="Q51" s="24"/>
+      <c r="R51" s="24"/>
+      <c r="S51" s="25"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="12"/>
-      <c r="K52" s="12"/>
-      <c r="L52" s="12"/>
-      <c r="M52" s="12"/>
-      <c r="N52" s="12"/>
-      <c r="O52" s="12"/>
-      <c r="P52" s="12"/>
-      <c r="Q52" s="12"/>
-      <c r="R52" s="12"/>
-      <c r="S52" s="13"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="19"/>
+      <c r="O52" s="19"/>
+      <c r="P52" s="19"/>
+      <c r="Q52" s="19"/>
+      <c r="R52" s="19"/>
+      <c r="S52" s="20"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="12"/>
-      <c r="L53" s="12"/>
-      <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
-      <c r="O53" s="12"/>
-      <c r="P53" s="12"/>
-      <c r="Q53" s="12"/>
-      <c r="R53" s="12"/>
-      <c r="S53" s="13"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
+      <c r="L53" s="19"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="19"/>
+      <c r="O53" s="19"/>
+      <c r="P53" s="19"/>
+      <c r="Q53" s="19"/>
+      <c r="R53" s="19"/>
+      <c r="S53" s="20"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="12"/>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
-      <c r="O54" s="12"/>
-      <c r="P54" s="12"/>
-      <c r="Q54" s="12"/>
-      <c r="R54" s="12"/>
-      <c r="S54" s="13"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="19"/>
+      <c r="M54" s="19"/>
+      <c r="N54" s="19"/>
+      <c r="O54" s="19"/>
+      <c r="P54" s="19"/>
+      <c r="Q54" s="19"/>
+      <c r="R54" s="19"/>
+      <c r="S54" s="20"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="12"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
-      <c r="O55" s="12"/>
-      <c r="P55" s="12"/>
-      <c r="Q55" s="12"/>
-      <c r="R55" s="12"/>
-      <c r="S55" s="13"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+      <c r="L55" s="19"/>
+      <c r="M55" s="19"/>
+      <c r="N55" s="19"/>
+      <c r="O55" s="19"/>
+      <c r="P55" s="19"/>
+      <c r="Q55" s="19"/>
+      <c r="R55" s="19"/>
+      <c r="S55" s="20"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14"/>
-      <c r="N56" s="14"/>
-      <c r="O56" s="14"/>
-      <c r="P56" s="14"/>
-      <c r="Q56" s="14"/>
-      <c r="R56" s="14"/>
-      <c r="S56" s="15"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="21"/>
+      <c r="N56" s="21"/>
+      <c r="O56" s="21"/>
+      <c r="P56" s="21"/>
+      <c r="Q56" s="21"/>
+      <c r="R56" s="21"/>
+      <c r="S56" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="A1:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A16:S17"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="J18:S18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="J20:S20"/>
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="J24:S24"/>
-    <mergeCell ref="J25:S25"/>
-    <mergeCell ref="J26:S26"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J27:S27"/>
-    <mergeCell ref="J28:S28"/>
-    <mergeCell ref="J29:S29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="J30:S30"/>
-    <mergeCell ref="J31:S31"/>
-    <mergeCell ref="J32:S32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="J34:S34"/>
-    <mergeCell ref="J35:S35"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B54:S54"/>
+    <mergeCell ref="B55:S55"/>
+    <mergeCell ref="B56:S56"/>
+    <mergeCell ref="J48:S48"/>
+    <mergeCell ref="A50:S50"/>
+    <mergeCell ref="B51:S51"/>
+    <mergeCell ref="B52:S52"/>
+    <mergeCell ref="B53:S53"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="J47:S47"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
     <mergeCell ref="J45:S45"/>
     <mergeCell ref="J46:S46"/>
     <mergeCell ref="B45:H45"/>
@@ -3132,24 +3229,48 @@
     <mergeCell ref="J42:S42"/>
     <mergeCell ref="J43:S43"/>
     <mergeCell ref="J44:S44"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B54:S54"/>
-    <mergeCell ref="B55:S55"/>
-    <mergeCell ref="B56:S56"/>
-    <mergeCell ref="J48:S48"/>
-    <mergeCell ref="A50:S50"/>
-    <mergeCell ref="B51:S51"/>
-    <mergeCell ref="B52:S52"/>
-    <mergeCell ref="B53:S53"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="J47:S47"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="J34:S34"/>
+    <mergeCell ref="J35:S35"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="J30:S30"/>
+    <mergeCell ref="J31:S31"/>
+    <mergeCell ref="J32:S32"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J27:S27"/>
+    <mergeCell ref="J28:S28"/>
+    <mergeCell ref="J29:S29"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J24:S24"/>
+    <mergeCell ref="J25:S25"/>
+    <mergeCell ref="J26:S26"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="J22:S22"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="J18:S18"/>
+    <mergeCell ref="J19:S19"/>
+    <mergeCell ref="J20:S20"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A16:S17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3157,6 +3278,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7005DF65C69D244A0053930B4D80895" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfe4224a46d45a1569ee43293fdcdd48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a217f1db-afc0-486b-a03f-32483c6d35f7" xmlns:ns4="b3fc9c33-149f-45e5-9bdb-a4f7fe310215" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d8dd93a9b58d240e8e3304885c0c0fa" ns3:_="" ns4:_="">
     <xsd:import namespace="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
@@ -3373,12 +3500,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3389,6 +3510,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D0DA503-506E-48B5-9538-4DAB746C5D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3407,23 +3545,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916385B-7771-4B86-AC30-95BD0DD5FA1F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Implemented new tab under product tab in main_form.py and ability to load picture files
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8485949-E43A-4A4D-B30D-AD752815D3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9664FDA8-C5A1-4F97-B2BD-539061119A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>NAPREDNE TEHNIKE PROGRAMIRANJA</t>
   </si>
@@ -174,25 +174,6 @@
   </si>
   <si>
     <t>Opis (polje ostavite prazno ako se funkcionalnost ne koristi u projektu)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* nazive dijaloga i njhovu svrhu unutar aplikacije (čemu služe)</t>
-    </r>
   </si>
   <si>
     <t>Svaka funkcionalnost treba biti odabrana i implementirana na način da je barem minimalno korisna u rješavanju problematike kojom se bavi vaša aplikacija. One funkcionalnosti koje ne doprinose izvornoj namjeni aplikacije ili njenim dijelovima neće biti uvažene.</t>
@@ -1070,6 +1051,60 @@
       <t xml:space="preserve">
 </t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* nazive dijaloga i njhovu svrhu unutar aplikacije (čemu služe)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Matija komentar:
+Komunikaija između dva dijaloga:
+Aplikacija se se sastoji od sljedecih forma:
+1. Forma za prijavu korisnika (login_form.py)
+Korisnik unosi username i password za login. Ako unese ispravne podatke login prođe, ako ne korisnik dobije poruku da je unesena krivi username ili password. Također na formi za prijavu korisnik može izabrati neki od ponuđena jezika na koji želi da mu se aplikacija prevede.
+2. Forma za CRUD operacije nad korisnicima (create_user_form.py)
+Button 'User Management' se nalazi na formi za prijavu korisnika. Klikom na button se otvara forma za
+CRUD operacije nad bazom podataka korisnika aplikacije
+3. Forma za CRUD operacije nad tablicama za pohranu dućana/skladista i proizvoda (main_form.py)
+ Ova forma služi za CRUD operacije nad tablicama skladista i proizvodi. Sluzi kako bi korisnik mogao dodati nova skladista i proizvode u bazu. Također se mogu pretraživati svi proizvodi, sva skladista, skladista u kojima se nallazi proizvod i slićno. </t>
+    </r>
+  </si>
+  <si>
+    <t>Trenutno 3 forma + komunikacija između dvije. Aplikacija će imati jos formi</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +1200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1191,6 +1226,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1371,7 +1412,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1400,6 +1441,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1427,6 +1474,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1449,20 +1505,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1780,1418 +1827,1422 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
-  <dimension ref="A1:S56"/>
+  <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25:S25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="20" max="20" width="68.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
+      <c r="A7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-    </row>
-    <row r="17" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-    </row>
-    <row r="18" spans="1:19" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+    </row>
+    <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+    </row>
+    <row r="18" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-    </row>
-    <row r="19" spans="1:19" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+    </row>
+    <row r="19" spans="1:20" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-    </row>
-    <row r="20" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="J19" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+    </row>
+    <row r="20" spans="1:20" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="32">
         <v>2</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-    </row>
-    <row r="21" spans="1:19" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>3</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-    </row>
-    <row r="22" spans="1:19" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31">
+      <c r="J21" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+    </row>
+    <row r="22" spans="1:20" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
         <v>4</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="B22" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-    </row>
-    <row r="23" spans="1:19" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+    </row>
+    <row r="23" spans="1:20" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="B23" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-    </row>
-    <row r="24" spans="1:19" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+    </row>
+    <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>6</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
-    </row>
-    <row r="25" spans="1:19" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27">
+      <c r="J24" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+    </row>
+    <row r="25" spans="1:20" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
         <v>7</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="29"/>
-      <c r="Q25" s="29"/>
-      <c r="R25" s="29"/>
-      <c r="S25" s="30"/>
-    </row>
-    <row r="26" spans="1:19" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="23"/>
+    </row>
+    <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>8</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-    </row>
-    <row r="27" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
+    </row>
+    <row r="27" spans="1:20" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>9</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-    </row>
-    <row r="28" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+    </row>
+    <row r="28" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>10</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="B28" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-    </row>
-    <row r="29" spans="1:19" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J28" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+    </row>
+    <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>11</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="B29" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="18"/>
-    </row>
-    <row r="30" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="20"/>
+    </row>
+    <row r="30" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>12</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
-    </row>
-    <row r="31" spans="1:19" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+    </row>
+    <row r="31" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="B31" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="15"/>
-    </row>
-    <row r="32" spans="1:19" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+    </row>
+    <row r="32" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>14</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
+      <c r="J32" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
+      <c r="B33" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="15"/>
+      <c r="J33" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
+      <c r="B34" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="15"/>
+      <c r="J34" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="17"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>17</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="15"/>
+      <c r="J35" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="17"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>18</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
+      <c r="J36" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
+      <c r="B37" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
+      <c r="J37" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="R37" s="17"/>
+      <c r="S37" s="17"/>
     </row>
     <row r="38" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>20</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
+      <c r="J38" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="17"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
-      <c r="B39" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
+      <c r="B39" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
-      <c r="P39" s="15"/>
-      <c r="Q39" s="15"/>
-      <c r="R39" s="15"/>
-      <c r="S39" s="15"/>
+      <c r="J39" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>22</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="15"/>
-      <c r="S40" s="15"/>
+      <c r="J40" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17"/>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="17"/>
+      <c r="S40" s="17"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-      <c r="S41" s="15"/>
+      <c r="J41" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="17"/>
+      <c r="S41" s="17"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="15"/>
-      <c r="S42" s="15"/>
+      <c r="J42" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="17"/>
+      <c r="S42" s="17"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
+      <c r="B43" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
+      <c r="J43" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="17"/>
+      <c r="P43" s="17"/>
+      <c r="Q43" s="17"/>
+      <c r="R43" s="17"/>
+      <c r="S43" s="17"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
+      <c r="J44" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
+      <c r="Q44" s="17"/>
+      <c r="R44" s="17"/>
+      <c r="S44" s="17"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="15"/>
-      <c r="R45" s="15"/>
-      <c r="S45" s="15"/>
+      <c r="J45" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="17"/>
+      <c r="Q45" s="17"/>
+      <c r="R45" s="17"/>
+      <c r="S45" s="17"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
-      <c r="P46" s="15"/>
-      <c r="Q46" s="15"/>
-      <c r="R46" s="15"/>
-      <c r="S46" s="15"/>
+      <c r="J46" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="17"/>
+      <c r="R46" s="17"/>
+      <c r="S46" s="17"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="15"/>
-      <c r="S47" s="15"/>
+      <c r="J47" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
+      <c r="Q47" s="17"/>
+      <c r="R47" s="17"/>
+      <c r="S47" s="17"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="15"/>
-      <c r="R48" s="15"/>
-      <c r="S48" s="15"/>
+      <c r="J48" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+      <c r="Q48" s="17"/>
+      <c r="R48" s="17"/>
+      <c r="S48" s="17"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="23" t="s">
+      <c r="A50" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="23"/>
-      <c r="K50" s="23"/>
-      <c r="L50" s="23"/>
-      <c r="M50" s="23"/>
-      <c r="N50" s="23"/>
-      <c r="O50" s="23"/>
-      <c r="P50" s="23"/>
-      <c r="Q50" s="23"/>
-      <c r="R50" s="23"/>
-      <c r="S50" s="23"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="28"/>
+      <c r="K50" s="28"/>
+      <c r="L50" s="28"/>
+      <c r="M50" s="28"/>
+      <c r="N50" s="28"/>
+      <c r="O50" s="28"/>
+      <c r="P50" s="28"/>
+      <c r="Q50" s="28"/>
+      <c r="R50" s="28"/>
+      <c r="S50" s="28"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
-      <c r="J51" s="24"/>
-      <c r="K51" s="24"/>
-      <c r="L51" s="24"/>
-      <c r="M51" s="24"/>
-      <c r="N51" s="24"/>
-      <c r="O51" s="24"/>
-      <c r="P51" s="24"/>
-      <c r="Q51" s="24"/>
-      <c r="R51" s="24"/>
-      <c r="S51" s="25"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="29"/>
+      <c r="K51" s="29"/>
+      <c r="L51" s="29"/>
+      <c r="M51" s="29"/>
+      <c r="N51" s="29"/>
+      <c r="O51" s="29"/>
+      <c r="P51" s="29"/>
+      <c r="Q51" s="29"/>
+      <c r="R51" s="29"/>
+      <c r="S51" s="30"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="19"/>
-      <c r="K52" s="19"/>
-      <c r="L52" s="19"/>
-      <c r="M52" s="19"/>
-      <c r="N52" s="19"/>
-      <c r="O52" s="19"/>
-      <c r="P52" s="19"/>
-      <c r="Q52" s="19"/>
-      <c r="R52" s="19"/>
-      <c r="S52" s="20"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="24"/>
+      <c r="J52" s="24"/>
+      <c r="K52" s="24"/>
+      <c r="L52" s="24"/>
+      <c r="M52" s="24"/>
+      <c r="N52" s="24"/>
+      <c r="O52" s="24"/>
+      <c r="P52" s="24"/>
+      <c r="Q52" s="24"/>
+      <c r="R52" s="24"/>
+      <c r="S52" s="25"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
-      <c r="J53" s="19"/>
-      <c r="K53" s="19"/>
-      <c r="L53" s="19"/>
-      <c r="M53" s="19"/>
-      <c r="N53" s="19"/>
-      <c r="O53" s="19"/>
-      <c r="P53" s="19"/>
-      <c r="Q53" s="19"/>
-      <c r="R53" s="19"/>
-      <c r="S53" s="20"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="24"/>
+      <c r="J53" s="24"/>
+      <c r="K53" s="24"/>
+      <c r="L53" s="24"/>
+      <c r="M53" s="24"/>
+      <c r="N53" s="24"/>
+      <c r="O53" s="24"/>
+      <c r="P53" s="24"/>
+      <c r="Q53" s="24"/>
+      <c r="R53" s="24"/>
+      <c r="S53" s="25"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
-      <c r="J54" s="19"/>
-      <c r="K54" s="19"/>
-      <c r="L54" s="19"/>
-      <c r="M54" s="19"/>
-      <c r="N54" s="19"/>
-      <c r="O54" s="19"/>
-      <c r="P54" s="19"/>
-      <c r="Q54" s="19"/>
-      <c r="R54" s="19"/>
-      <c r="S54" s="20"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24"/>
+      <c r="K54" s="24"/>
+      <c r="L54" s="24"/>
+      <c r="M54" s="24"/>
+      <c r="N54" s="24"/>
+      <c r="O54" s="24"/>
+      <c r="P54" s="24"/>
+      <c r="Q54" s="24"/>
+      <c r="R54" s="24"/>
+      <c r="S54" s="25"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19"/>
-      <c r="J55" s="19"/>
-      <c r="K55" s="19"/>
-      <c r="L55" s="19"/>
-      <c r="M55" s="19"/>
-      <c r="N55" s="19"/>
-      <c r="O55" s="19"/>
-      <c r="P55" s="19"/>
-      <c r="Q55" s="19"/>
-      <c r="R55" s="19"/>
-      <c r="S55" s="20"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="24"/>
+      <c r="J55" s="24"/>
+      <c r="K55" s="24"/>
+      <c r="L55" s="24"/>
+      <c r="M55" s="24"/>
+      <c r="N55" s="24"/>
+      <c r="O55" s="24"/>
+      <c r="P55" s="24"/>
+      <c r="Q55" s="24"/>
+      <c r="R55" s="24"/>
+      <c r="S55" s="25"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="21"/>
-      <c r="M56" s="21"/>
-      <c r="N56" s="21"/>
-      <c r="O56" s="21"/>
-      <c r="P56" s="21"/>
-      <c r="Q56" s="21"/>
-      <c r="R56" s="21"/>
-      <c r="S56" s="22"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="26"/>
+      <c r="L56" s="26"/>
+      <c r="M56" s="26"/>
+      <c r="N56" s="26"/>
+      <c r="O56" s="26"/>
+      <c r="P56" s="26"/>
+      <c r="Q56" s="26"/>
+      <c r="R56" s="26"/>
+      <c r="S56" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="76">

</xml_diff>

<commit_message>
Implemented ability to import and show pictures from databaze
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9664FDA8-C5A1-4F97-B2BD-539061119A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841FB4F4-8C71-48FD-8331-299C9740642E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -556,25 +556,6 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* kakav se sadržaj nalazi u blob polju te koje od operacija su nad njim podržane unutar aplikacije</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>* koji su sve jezici podržani</t>
     </r>
     <r>
@@ -1105,6 +1086,49 @@
   </si>
   <si>
     <t>Trenutno 3 forma + komunikacija između dvije. Aplikacija će imati jos formi</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* kakav se sadržaj nalazi u blob polju te koje od operacija su nad njim podržane unutar aplikacije</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija komentar:
+U MS Access bazi podataka skladiste, tablica proizvodi, stupac privitak sadrži binarny sadržaj tipa OLE Object, tj. binarno zapisana slika proizvoda.
+U aplikaciji se po proizvod_id moze dodati tabu 'Add/Show product picture' moze dodati i prikazati slika iz base podataka.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1447,40 +1471,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1505,11 +1505,35 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1830,7 +1854,7 @@
   <dimension ref="A1:T56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,1429 +1865,1453 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
+      <c r="A7" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="31"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="33"/>
     </row>
     <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="33"/>
     </row>
     <row r="18" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
     </row>
     <row r="19" spans="1:20" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J19" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
     </row>
     <row r="20" spans="1:20" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32">
+      <c r="A20" s="12">
         <v>2</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="17" t="s">
+      <c r="J20" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="33" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>3</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
+      <c r="J21" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
     </row>
     <row r="22" spans="1:20" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>4</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
+      <c r="B22" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
+      <c r="J22" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
     </row>
     <row r="23" spans="1:20" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
+      <c r="B23" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
+      <c r="J23" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
     </row>
     <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>6</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
+      <c r="J24" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
     </row>
     <row r="25" spans="1:20" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>7</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="22"/>
-      <c r="S25" s="23"/>
+      <c r="J25" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="27"/>
     </row>
     <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>8</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="17"/>
-      <c r="S26" s="17"/>
-    </row>
-    <row r="27" spans="1:20" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="J26" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+    </row>
+    <row r="27" spans="1:20" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
         <v>9</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="17"/>
+      <c r="J27" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
     </row>
     <row r="28" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>10</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
+      <c r="B28" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="17" t="s">
+      <c r="J28" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="17"/>
-      <c r="S28" s="17"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
     </row>
     <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>11</v>
       </c>
-      <c r="B29" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
+      <c r="B29" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="20"/>
-      <c r="R29" s="20"/>
-      <c r="S29" s="20"/>
+      <c r="J29" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="24"/>
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
     </row>
     <row r="30" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>12</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="17" t="s">
+      <c r="J30" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="17"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
     </row>
     <row r="31" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
+      <c r="B31" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="17" t="s">
+      <c r="J31" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
     </row>
     <row r="32" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>14</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="17" t="s">
+      <c r="J32" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="17"/>
-      <c r="S32" s="17"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
+      <c r="B33" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="17" t="s">
+      <c r="J33" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="17"/>
-      <c r="N33" s="17"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="17"/>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="17"/>
-      <c r="S33" s="17"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
+      <c r="B34" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="17" t="s">
+      <c r="J34" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17"/>
-      <c r="Q34" s="17"/>
-      <c r="R34" s="17"/>
-      <c r="S34" s="17"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>17</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="17" t="s">
+      <c r="J35" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17"/>
-      <c r="O35" s="17"/>
-      <c r="P35" s="17"/>
-      <c r="Q35" s="17"/>
-      <c r="R35" s="17"/>
-      <c r="S35" s="17"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>18</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="17" t="s">
+      <c r="J36" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17"/>
-      <c r="O36" s="17"/>
-      <c r="P36" s="17"/>
-      <c r="Q36" s="17"/>
-      <c r="R36" s="17"/>
-      <c r="S36" s="17"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
+      <c r="B37" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="17" t="s">
+      <c r="J37" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
-      <c r="Q37" s="17"/>
-      <c r="R37" s="17"/>
-      <c r="S37" s="17"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
     </row>
     <row r="38" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>20</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="17" t="s">
+      <c r="J38" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17"/>
-      <c r="Q38" s="17"/>
-      <c r="R38" s="17"/>
-      <c r="S38" s="17"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
-      <c r="B39" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
+      <c r="B39" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="17"/>
-      <c r="P39" s="17"/>
-      <c r="Q39" s="17"/>
-      <c r="R39" s="17"/>
-      <c r="S39" s="17"/>
+      <c r="J39" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="15"/>
+      <c r="S39" s="15"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>22</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="17" t="s">
+      <c r="J40" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="17"/>
-      <c r="O40" s="17"/>
-      <c r="P40" s="17"/>
-      <c r="Q40" s="17"/>
-      <c r="R40" s="17"/>
-      <c r="S40" s="17"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="K41" s="17"/>
-      <c r="L41" s="17"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="17"/>
-      <c r="O41" s="17"/>
-      <c r="P41" s="17"/>
-      <c r="Q41" s="17"/>
-      <c r="R41" s="17"/>
-      <c r="S41" s="17"/>
+      <c r="J41" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
+      <c r="S41" s="15"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="K42" s="17"/>
-      <c r="L42" s="17"/>
-      <c r="M42" s="17"/>
-      <c r="N42" s="17"/>
-      <c r="O42" s="17"/>
-      <c r="P42" s="17"/>
-      <c r="Q42" s="17"/>
-      <c r="R42" s="17"/>
-      <c r="S42" s="17"/>
+      <c r="J42" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="15"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
+      <c r="B43" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="K43" s="17"/>
-      <c r="L43" s="17"/>
-      <c r="M43" s="17"/>
-      <c r="N43" s="17"/>
-      <c r="O43" s="17"/>
-      <c r="P43" s="17"/>
-      <c r="Q43" s="17"/>
-      <c r="R43" s="17"/>
-      <c r="S43" s="17"/>
+      <c r="J43" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="15"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="17" t="s">
+      <c r="J44" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="K44" s="17"/>
-      <c r="L44" s="17"/>
-      <c r="M44" s="17"/>
-      <c r="N44" s="17"/>
-      <c r="O44" s="17"/>
-      <c r="P44" s="17"/>
-      <c r="Q44" s="17"/>
-      <c r="R44" s="17"/>
-      <c r="S44" s="17"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="17" t="s">
+      <c r="J45" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="K45" s="17"/>
-      <c r="L45" s="17"/>
-      <c r="M45" s="17"/>
-      <c r="N45" s="17"/>
-      <c r="O45" s="17"/>
-      <c r="P45" s="17"/>
-      <c r="Q45" s="17"/>
-      <c r="R45" s="17"/>
-      <c r="S45" s="17"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
+      <c r="S45" s="15"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="17" t="s">
+      <c r="J46" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="K46" s="17"/>
-      <c r="L46" s="17"/>
-      <c r="M46" s="17"/>
-      <c r="N46" s="17"/>
-      <c r="O46" s="17"/>
-      <c r="P46" s="17"/>
-      <c r="Q46" s="17"/>
-      <c r="R46" s="17"/>
-      <c r="S46" s="17"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+      <c r="R46" s="15"/>
+      <c r="S46" s="15"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="17" t="s">
+      <c r="J47" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="K47" s="17"/>
-      <c r="L47" s="17"/>
-      <c r="M47" s="17"/>
-      <c r="N47" s="17"/>
-      <c r="O47" s="17"/>
-      <c r="P47" s="17"/>
-      <c r="Q47" s="17"/>
-      <c r="R47" s="17"/>
-      <c r="S47" s="17"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="15"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="17" t="s">
+      <c r="J48" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="K48" s="17"/>
-      <c r="L48" s="17"/>
-      <c r="M48" s="17"/>
-      <c r="N48" s="17"/>
-      <c r="O48" s="17"/>
-      <c r="P48" s="17"/>
-      <c r="Q48" s="17"/>
-      <c r="R48" s="17"/>
-      <c r="S48" s="17"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
+      <c r="S48" s="15"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="31"/>
-      <c r="H49" s="31"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
+      <c r="A50" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="28"/>
-      <c r="J50" s="28"/>
-      <c r="K50" s="28"/>
-      <c r="L50" s="28"/>
-      <c r="M50" s="28"/>
-      <c r="N50" s="28"/>
-      <c r="O50" s="28"/>
-      <c r="P50" s="28"/>
-      <c r="Q50" s="28"/>
-      <c r="R50" s="28"/>
-      <c r="S50" s="28"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="20"/>
+      <c r="O50" s="20"/>
+      <c r="P50" s="20"/>
+      <c r="Q50" s="20"/>
+      <c r="R50" s="20"/>
+      <c r="S50" s="20"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="29"/>
-      <c r="I51" s="29"/>
-      <c r="J51" s="29"/>
-      <c r="K51" s="29"/>
-      <c r="L51" s="29"/>
-      <c r="M51" s="29"/>
-      <c r="N51" s="29"/>
-      <c r="O51" s="29"/>
-      <c r="P51" s="29"/>
-      <c r="Q51" s="29"/>
-      <c r="R51" s="29"/>
-      <c r="S51" s="30"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="21"/>
+      <c r="O51" s="21"/>
+      <c r="P51" s="21"/>
+      <c r="Q51" s="21"/>
+      <c r="R51" s="21"/>
+      <c r="S51" s="22"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
-      <c r="K52" s="24"/>
-      <c r="L52" s="24"/>
-      <c r="M52" s="24"/>
-      <c r="N52" s="24"/>
-      <c r="O52" s="24"/>
-      <c r="P52" s="24"/>
-      <c r="Q52" s="24"/>
-      <c r="R52" s="24"/>
-      <c r="S52" s="25"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="L52" s="16"/>
+      <c r="M52" s="16"/>
+      <c r="N52" s="16"/>
+      <c r="O52" s="16"/>
+      <c r="P52" s="16"/>
+      <c r="Q52" s="16"/>
+      <c r="R52" s="16"/>
+      <c r="S52" s="17"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="24"/>
-      <c r="I53" s="24"/>
-      <c r="J53" s="24"/>
-      <c r="K53" s="24"/>
-      <c r="L53" s="24"/>
-      <c r="M53" s="24"/>
-      <c r="N53" s="24"/>
-      <c r="O53" s="24"/>
-      <c r="P53" s="24"/>
-      <c r="Q53" s="24"/>
-      <c r="R53" s="24"/>
-      <c r="S53" s="25"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="16"/>
+      <c r="M53" s="16"/>
+      <c r="N53" s="16"/>
+      <c r="O53" s="16"/>
+      <c r="P53" s="16"/>
+      <c r="Q53" s="16"/>
+      <c r="R53" s="16"/>
+      <c r="S53" s="17"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="24"/>
-      <c r="I54" s="24"/>
-      <c r="J54" s="24"/>
-      <c r="K54" s="24"/>
-      <c r="L54" s="24"/>
-      <c r="M54" s="24"/>
-      <c r="N54" s="24"/>
-      <c r="O54" s="24"/>
-      <c r="P54" s="24"/>
-      <c r="Q54" s="24"/>
-      <c r="R54" s="24"/>
-      <c r="S54" s="25"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="16"/>
+      <c r="O54" s="16"/>
+      <c r="P54" s="16"/>
+      <c r="Q54" s="16"/>
+      <c r="R54" s="16"/>
+      <c r="S54" s="17"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="24"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="24"/>
-      <c r="J55" s="24"/>
-      <c r="K55" s="24"/>
-      <c r="L55" s="24"/>
-      <c r="M55" s="24"/>
-      <c r="N55" s="24"/>
-      <c r="O55" s="24"/>
-      <c r="P55" s="24"/>
-      <c r="Q55" s="24"/>
-      <c r="R55" s="24"/>
-      <c r="S55" s="25"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="16"/>
+      <c r="S55" s="17"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="26"/>
-      <c r="I56" s="26"/>
-      <c r="J56" s="26"/>
-      <c r="K56" s="26"/>
-      <c r="L56" s="26"/>
-      <c r="M56" s="26"/>
-      <c r="N56" s="26"/>
-      <c r="O56" s="26"/>
-      <c r="P56" s="26"/>
-      <c r="Q56" s="26"/>
-      <c r="R56" s="26"/>
-      <c r="S56" s="27"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="18"/>
+      <c r="P56" s="18"/>
+      <c r="Q56" s="18"/>
+      <c r="R56" s="18"/>
+      <c r="S56" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B54:S54"/>
-    <mergeCell ref="B55:S55"/>
-    <mergeCell ref="B56:S56"/>
-    <mergeCell ref="J48:S48"/>
-    <mergeCell ref="A50:S50"/>
-    <mergeCell ref="B51:S51"/>
-    <mergeCell ref="B52:S52"/>
-    <mergeCell ref="B53:S53"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="J47:S47"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="J22:S22"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="J18:S18"/>
+    <mergeCell ref="J19:S19"/>
+    <mergeCell ref="J20:S20"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J24:S24"/>
+    <mergeCell ref="J25:S25"/>
+    <mergeCell ref="J26:S26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J27:S27"/>
+    <mergeCell ref="J28:S28"/>
+    <mergeCell ref="J29:S29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="J30:S30"/>
+    <mergeCell ref="J31:S31"/>
+    <mergeCell ref="J32:S32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="J34:S34"/>
+    <mergeCell ref="J35:S35"/>
     <mergeCell ref="J45:S45"/>
     <mergeCell ref="J46:S46"/>
     <mergeCell ref="B45:H45"/>
@@ -3280,48 +3328,24 @@
     <mergeCell ref="J42:S42"/>
     <mergeCell ref="J43:S43"/>
     <mergeCell ref="J44:S44"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="J34:S34"/>
-    <mergeCell ref="J35:S35"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="J30:S30"/>
-    <mergeCell ref="J31:S31"/>
-    <mergeCell ref="J32:S32"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J27:S27"/>
-    <mergeCell ref="J28:S28"/>
-    <mergeCell ref="J29:S29"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="J24:S24"/>
-    <mergeCell ref="J25:S25"/>
-    <mergeCell ref="J26:S26"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="J18:S18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="J20:S20"/>
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="A1:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B54:S54"/>
+    <mergeCell ref="B55:S55"/>
+    <mergeCell ref="B56:S56"/>
+    <mergeCell ref="J48:S48"/>
+    <mergeCell ref="A50:S50"/>
+    <mergeCell ref="B51:S51"/>
+    <mergeCell ref="B52:S52"/>
+    <mergeCell ref="B53:S53"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="J47:S47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3329,12 +3353,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7005DF65C69D244A0053930B4D80895" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfe4224a46d45a1569ee43293fdcdd48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a217f1db-afc0-486b-a03f-32483c6d35f7" xmlns:ns4="b3fc9c33-149f-45e5-9bdb-a4f7fe310215" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d8dd93a9b58d240e8e3304885c0c0fa" ns3:_="" ns4:_="">
     <xsd:import namespace="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
@@ -3551,6 +3569,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3561,23 +3585,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D0DA503-506E-48B5-9538-4DAB746C5D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3596,6 +3603,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916385B-7771-4B86-AC30-95BD0DD5FA1F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
small changes all over the files
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841FB4F4-8C71-48FD-8331-299C9740642E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F979FFFB-19B4-4C10-A339-97508F36660F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>NAPREDNE TEHNIKE PROGRAMIRANJA</t>
   </si>
@@ -1049,6 +1049,49 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
+      <t>* kakav se sadržaj nalazi u blob polju te koje od operacija su nad njim podržane unutar aplikacije</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija komentar:
+U MS Access bazi podataka skladiste, tablica proizvodi, stupac privitak sadrži binarny sadržaj tipa OLE Object, tj. binarno zapisana slika proizvoda.
+U aplikaciji se po proizvod_id moze dodati tabu 'Add/Show product picture' moze dodati i prikazati slika iz base podataka.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">* nazive dijaloga i njhovu svrhu unutar aplikacije (čemu služe)
 </t>
     </r>
@@ -1074,6 +1117,10 @@
       </rPr>
       <t xml:space="preserve">Matija komentar:
 Komunikaija između dva dijaloga:
+1.login_form.py -&gt; main_form.py
+Iz login_form.py se konstruktoru  main_form.py predaju dva podatka, username korisnika koji se ulogirao i jezik koji je odabrao prilikom logina. Ti podaci se na main_form.py u gornjem lijevom kutu prikazuju
+2. main_form.py -&gt; show_image_form.py
+Iz main_form.py prenosi se binarni zapis slike u konstruktor show_image_form.py kroz varijablu self.temp_blob_variable koja se unutar klase koristi za prikaz 
 Aplikacija se se sastoji od sljedecih forma:
 1. Forma za prijavu korisnika (login_form.py)
 Korisnik unosi username i password za login. Ako unese ispravne podatke login prođe, ako ne korisnik dobije poruku da je unesena krivi username ili password. Također na formi za prijavu korisnik može izabrati neki od ponuđena jezika na koji želi da mu se aplikacija prevede.
@@ -1081,29 +1128,7 @@
 Button 'User Management' se nalazi na formi za prijavu korisnika. Klikom na button se otvara forma za
 CRUD operacije nad bazom podataka korisnika aplikacije
 3. Forma za CRUD operacije nad tablicama za pohranu dućana/skladista i proizvoda (main_form.py)
- Ova forma služi za CRUD operacije nad tablicama skladista i proizvodi. Sluzi kako bi korisnik mogao dodati nova skladista i proizvode u bazu. Također se mogu pretraživati svi proizvodi, sva skladista, skladista u kojima se nallazi proizvod i slićno. </t>
-    </r>
-  </si>
-  <si>
-    <t>Trenutno 3 forma + komunikacija između dvije. Aplikacija će imati jos formi</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* kakav se sadržaj nalazi u blob polju te koje od operacija su nad njim podržane unutar aplikacije</t>
+Ova forma služi za CRUD operacije nad tablicama skladista i proizvodi. Sluzi kako bi korisnik mogao dodati nova skladista i proizvode u bazu. Također se mogu pretraživati svi proizvodi, sva skladista, skladista u kojima se nallazi proizvod i slićno. </t>
     </r>
     <r>
       <rPr>
@@ -1125,9 +1150,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Matija komentar:
-U MS Access bazi podataka skladiste, tablica proizvodi, stupac privitak sadrži binarny sadržaj tipa OLE Object, tj. binarno zapisana slika proizvoda.
-U aplikaciji se po proizvod_id moze dodati tabu 'Add/Show product picture' moze dodati i prikazati slika iz base podataka.</t>
+      <t>4. Forma za prikaz slike iz baze podataka (show_image_form.py)
+Ova forma sluzi za prikaz binarnog podatka (slike) iz baze podatka</t>
     </r>
   </si>
 </sst>
@@ -1224,7 +1248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1250,12 +1274,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1436,7 +1454,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1471,16 +1489,43 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1505,36 +1550,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1854,7 +1869,7 @@
   <dimension ref="A1:T56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="B28" sqref="B28:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1865,1453 +1880,1427 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="32"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="32"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="32"/>
-      <c r="S12" s="32"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="31"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="31"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="33"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
     </row>
     <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
-      <c r="Q17" s="33"/>
-      <c r="R17" s="33"/>
-      <c r="S17" s="33"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
     </row>
     <row r="18" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="29" t="s">
+      <c r="J18" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
     </row>
     <row r="19" spans="1:20" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="J19" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
     </row>
     <row r="20" spans="1:20" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="A20" s="10">
         <v>2</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="13" t="s">
+      <c r="J20" s="18" t="s">
         <v>69</v>
       </c>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="12"/>
     </row>
     <row r="21" spans="1:20" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>3</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="15" t="s">
+      <c r="J21" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
     </row>
     <row r="22" spans="1:20" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>4</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="15" t="s">
+      <c r="J22" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
     </row>
     <row r="23" spans="1:20" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="J23" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
     </row>
     <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>6</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="15" t="s">
+      <c r="J24" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
     </row>
     <row r="25" spans="1:20" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>7</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="25" t="s">
+      <c r="J25" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
-      <c r="S25" s="27"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="24"/>
     </row>
     <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>8</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="15" t="s">
+      <c r="J26" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
     </row>
     <row r="27" spans="1:20" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>9</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
+      <c r="J27" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
     </row>
     <row r="28" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>10</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="15" t="s">
+      <c r="J28" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
     </row>
     <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>11</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="15" t="s">
+      <c r="J29" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
     </row>
     <row r="30" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>12</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="15" t="s">
+      <c r="J30" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
     </row>
     <row r="31" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="15" t="s">
+      <c r="J31" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="15"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
     </row>
     <row r="32" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>14</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="15" t="s">
+      <c r="J32" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="15" t="s">
+      <c r="J33" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="15"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="15" t="s">
+      <c r="J34" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="15"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>17</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="15" t="s">
+      <c r="J35" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="15"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>18</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="15" t="s">
+      <c r="J36" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="15" t="s">
+      <c r="J37" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
     </row>
     <row r="38" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>20</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="15" t="s">
+      <c r="J38" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="18"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="15" t="s">
+      <c r="J39" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
-      <c r="P39" s="15"/>
-      <c r="Q39" s="15"/>
-      <c r="R39" s="15"/>
-      <c r="S39" s="15"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>22</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="15" t="s">
+      <c r="J40" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="15"/>
-      <c r="S40" s="15"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="15" t="s">
+      <c r="J41" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-      <c r="S41" s="15"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="15" t="s">
+      <c r="J42" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="15"/>
-      <c r="S42" s="15"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="18"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="15" t="s">
+      <c r="J43" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="15" t="s">
+      <c r="J44" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="15" t="s">
+      <c r="J45" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="15"/>
-      <c r="R45" s="15"/>
-      <c r="S45" s="15"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="15" t="s">
+      <c r="J46" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
-      <c r="P46" s="15"/>
-      <c r="Q46" s="15"/>
-      <c r="R46" s="15"/>
-      <c r="S46" s="15"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18"/>
+      <c r="S46" s="18"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="15" t="s">
+      <c r="J47" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="15"/>
-      <c r="S47" s="15"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="15" t="s">
+      <c r="J48" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="15"/>
-      <c r="R48" s="15"/>
-      <c r="S48" s="15"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="18"/>
+      <c r="S48" s="18"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
-      <c r="H49" s="23"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="20" t="s">
+      <c r="A50" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
-      <c r="O50" s="20"/>
-      <c r="P50" s="20"/>
-      <c r="Q50" s="20"/>
-      <c r="R50" s="20"/>
-      <c r="S50" s="20"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="29"/>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="29"/>
+      <c r="Q50" s="29"/>
+      <c r="R50" s="29"/>
+      <c r="S50" s="29"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="21"/>
-      <c r="K51" s="21"/>
-      <c r="L51" s="21"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="21"/>
-      <c r="O51" s="21"/>
-      <c r="P51" s="21"/>
-      <c r="Q51" s="21"/>
-      <c r="R51" s="21"/>
-      <c r="S51" s="22"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="30"/>
+      <c r="L51" s="30"/>
+      <c r="M51" s="30"/>
+      <c r="N51" s="30"/>
+      <c r="O51" s="30"/>
+      <c r="P51" s="30"/>
+      <c r="Q51" s="30"/>
+      <c r="R51" s="30"/>
+      <c r="S51" s="31"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16"/>
-      <c r="I52" s="16"/>
-      <c r="J52" s="16"/>
-      <c r="K52" s="16"/>
-      <c r="L52" s="16"/>
-      <c r="M52" s="16"/>
-      <c r="N52" s="16"/>
-      <c r="O52" s="16"/>
-      <c r="P52" s="16"/>
-      <c r="Q52" s="16"/>
-      <c r="R52" s="16"/>
-      <c r="S52" s="17"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="25"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="25"/>
+      <c r="N52" s="25"/>
+      <c r="O52" s="25"/>
+      <c r="P52" s="25"/>
+      <c r="Q52" s="25"/>
+      <c r="R52" s="25"/>
+      <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="16"/>
-      <c r="I53" s="16"/>
-      <c r="J53" s="16"/>
-      <c r="K53" s="16"/>
-      <c r="L53" s="16"/>
-      <c r="M53" s="16"/>
-      <c r="N53" s="16"/>
-      <c r="O53" s="16"/>
-      <c r="P53" s="16"/>
-      <c r="Q53" s="16"/>
-      <c r="R53" s="16"/>
-      <c r="S53" s="17"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="25"/>
+      <c r="O53" s="25"/>
+      <c r="P53" s="25"/>
+      <c r="Q53" s="25"/>
+      <c r="R53" s="25"/>
+      <c r="S53" s="26"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="16"/>
-      <c r="I54" s="16"/>
-      <c r="J54" s="16"/>
-      <c r="K54" s="16"/>
-      <c r="L54" s="16"/>
-      <c r="M54" s="16"/>
-      <c r="N54" s="16"/>
-      <c r="O54" s="16"/>
-      <c r="P54" s="16"/>
-      <c r="Q54" s="16"/>
-      <c r="R54" s="16"/>
-      <c r="S54" s="17"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="25"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="25"/>
+      <c r="N54" s="25"/>
+      <c r="O54" s="25"/>
+      <c r="P54" s="25"/>
+      <c r="Q54" s="25"/>
+      <c r="R54" s="25"/>
+      <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="16"/>
-      <c r="I55" s="16"/>
-      <c r="J55" s="16"/>
-      <c r="K55" s="16"/>
-      <c r="L55" s="16"/>
-      <c r="M55" s="16"/>
-      <c r="N55" s="16"/>
-      <c r="O55" s="16"/>
-      <c r="P55" s="16"/>
-      <c r="Q55" s="16"/>
-      <c r="R55" s="16"/>
-      <c r="S55" s="17"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="25"/>
+      <c r="K55" s="25"/>
+      <c r="L55" s="25"/>
+      <c r="M55" s="25"/>
+      <c r="N55" s="25"/>
+      <c r="O55" s="25"/>
+      <c r="P55" s="25"/>
+      <c r="Q55" s="25"/>
+      <c r="R55" s="25"/>
+      <c r="S55" s="26"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18"/>
-      <c r="L56" s="18"/>
-      <c r="M56" s="18"/>
-      <c r="N56" s="18"/>
-      <c r="O56" s="18"/>
-      <c r="P56" s="18"/>
-      <c r="Q56" s="18"/>
-      <c r="R56" s="18"/>
-      <c r="S56" s="19"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="27"/>
+      <c r="J56" s="27"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="27"/>
+      <c r="M56" s="27"/>
+      <c r="N56" s="27"/>
+      <c r="O56" s="27"/>
+      <c r="P56" s="27"/>
+      <c r="Q56" s="27"/>
+      <c r="R56" s="27"/>
+      <c r="S56" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="A1:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A16:S17"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="J18:S18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="J20:S20"/>
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="J24:S24"/>
-    <mergeCell ref="J25:S25"/>
-    <mergeCell ref="J26:S26"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J27:S27"/>
-    <mergeCell ref="J28:S28"/>
-    <mergeCell ref="J29:S29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="J30:S30"/>
-    <mergeCell ref="J31:S31"/>
-    <mergeCell ref="J32:S32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="J34:S34"/>
-    <mergeCell ref="J35:S35"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B54:S54"/>
+    <mergeCell ref="B55:S55"/>
+    <mergeCell ref="B56:S56"/>
+    <mergeCell ref="J48:S48"/>
+    <mergeCell ref="A50:S50"/>
+    <mergeCell ref="B51:S51"/>
+    <mergeCell ref="B52:S52"/>
+    <mergeCell ref="B53:S53"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="J47:S47"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
     <mergeCell ref="J45:S45"/>
     <mergeCell ref="J46:S46"/>
     <mergeCell ref="B45:H45"/>
@@ -3328,24 +3317,48 @@
     <mergeCell ref="J42:S42"/>
     <mergeCell ref="J43:S43"/>
     <mergeCell ref="J44:S44"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B54:S54"/>
-    <mergeCell ref="B55:S55"/>
-    <mergeCell ref="B56:S56"/>
-    <mergeCell ref="J48:S48"/>
-    <mergeCell ref="A50:S50"/>
-    <mergeCell ref="B51:S51"/>
-    <mergeCell ref="B52:S52"/>
-    <mergeCell ref="B53:S53"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="J47:S47"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="J34:S34"/>
+    <mergeCell ref="J35:S35"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="J30:S30"/>
+    <mergeCell ref="J31:S31"/>
+    <mergeCell ref="J32:S32"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J27:S27"/>
+    <mergeCell ref="J28:S28"/>
+    <mergeCell ref="J29:S29"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J24:S24"/>
+    <mergeCell ref="J25:S25"/>
+    <mergeCell ref="J26:S26"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="J22:S22"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="J18:S18"/>
+    <mergeCell ref="J19:S19"/>
+    <mergeCell ref="J20:S20"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A16:S17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3353,6 +3366,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7005DF65C69D244A0053930B4D80895" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfe4224a46d45a1569ee43293fdcdd48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a217f1db-afc0-486b-a03f-32483c6d35f7" xmlns:ns4="b3fc9c33-149f-45e5-9bdb-a4f7fe310215" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d8dd93a9b58d240e8e3304885c0c0fa" ns3:_="" ns4:_="">
     <xsd:import namespace="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
@@ -3569,12 +3588,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3585,6 +3598,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D0DA503-506E-48B5-9538-4DAB746C5D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3603,23 +3633,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916385B-7771-4B86-AC30-95BD0DD5FA1F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Implemented ability to generate 2 reports in .rtf format. One for table products, and another one for master-detail relationship on table warehouse->products
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F979FFFB-19B4-4C10-A339-97508F36660F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF788C8-5D02-428B-9769-851E26327387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -1492,40 +1492,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1550,6 +1520,36 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1880,1427 +1880,1451 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
     </row>
     <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
     </row>
     <row r="18" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="20" t="s">
+      <c r="J18" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
     </row>
     <row r="19" spans="1:20" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="18" t="s">
+      <c r="J19" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
     </row>
     <row r="20" spans="1:20" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="J20" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
       <c r="T20" s="12"/>
     </row>
     <row r="21" spans="1:20" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>3</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="18" t="s">
+      <c r="J21" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
     </row>
     <row r="22" spans="1:20" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>4</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="18" t="s">
+      <c r="J22" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
     </row>
     <row r="23" spans="1:20" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="18" t="s">
+      <c r="J23" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
     </row>
     <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>6</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="18" t="s">
+      <c r="J24" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
     </row>
     <row r="25" spans="1:20" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>7</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="22" t="s">
+      <c r="J25" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="24"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>8</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="18" t="s">
+      <c r="J26" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
     </row>
     <row r="27" spans="1:20" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>9</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="18" t="s">
+      <c r="J27" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
     </row>
     <row r="28" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>10</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="18" t="s">
+      <c r="J28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
     </row>
     <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>11</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="18" t="s">
+      <c r="J29" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="21"/>
-      <c r="S29" s="21"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
     </row>
     <row r="30" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>12</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="18" t="s">
+      <c r="J30" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
     </row>
     <row r="31" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="18" t="s">
+      <c r="J31" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
     </row>
     <row r="32" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>14</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="18" t="s">
+      <c r="J32" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="18" t="s">
+      <c r="J33" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="18" t="s">
+      <c r="J34" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>17</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="18" t="s">
+      <c r="J35" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>18</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="18" t="s">
+      <c r="J36" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="18"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="18" t="s">
+      <c r="J37" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
     </row>
     <row r="38" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>20</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="18" t="s">
+      <c r="J38" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="18" t="s">
+      <c r="J39" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>22</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="18" t="s">
+      <c r="J40" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="18" t="s">
+      <c r="J41" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="18" t="s">
+      <c r="J42" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="18" t="s">
+      <c r="J43" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="18" t="s">
+      <c r="J44" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="18" t="s">
+      <c r="J45" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="18" t="s">
+      <c r="J46" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="14"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="18" t="s">
+      <c r="J47" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="18" t="s">
+      <c r="J48" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="18"/>
-      <c r="O48" s="18"/>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="18"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
-      <c r="N50" s="29"/>
-      <c r="O50" s="29"/>
-      <c r="P50" s="29"/>
-      <c r="Q50" s="29"/>
-      <c r="R50" s="29"/>
-      <c r="S50" s="29"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="30"/>
-      <c r="M51" s="30"/>
-      <c r="N51" s="30"/>
-      <c r="O51" s="30"/>
-      <c r="P51" s="30"/>
-      <c r="Q51" s="30"/>
-      <c r="R51" s="30"/>
-      <c r="S51" s="31"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="20"/>
+      <c r="O51" s="20"/>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="20"/>
+      <c r="S51" s="21"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="25"/>
-      <c r="L52" s="25"/>
-      <c r="M52" s="25"/>
-      <c r="N52" s="25"/>
-      <c r="O52" s="25"/>
-      <c r="P52" s="25"/>
-      <c r="Q52" s="25"/>
-      <c r="R52" s="25"/>
-      <c r="S52" s="26"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="15"/>
+      <c r="O52" s="15"/>
+      <c r="P52" s="15"/>
+      <c r="Q52" s="15"/>
+      <c r="R52" s="15"/>
+      <c r="S52" s="16"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
-      <c r="O53" s="25"/>
-      <c r="P53" s="25"/>
-      <c r="Q53" s="25"/>
-      <c r="R53" s="25"/>
-      <c r="S53" s="26"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="15"/>
+      <c r="S53" s="16"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
-      <c r="L54" s="25"/>
-      <c r="M54" s="25"/>
-      <c r="N54" s="25"/>
-      <c r="O54" s="25"/>
-      <c r="P54" s="25"/>
-      <c r="Q54" s="25"/>
-      <c r="R54" s="25"/>
-      <c r="S54" s="26"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+      <c r="S54" s="16"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="25"/>
-      <c r="L55" s="25"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="25"/>
-      <c r="O55" s="25"/>
-      <c r="P55" s="25"/>
-      <c r="Q55" s="25"/>
-      <c r="R55" s="25"/>
-      <c r="S55" s="26"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="15"/>
+      <c r="R55" s="15"/>
+      <c r="S55" s="16"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="27"/>
-      <c r="J56" s="27"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="27"/>
-      <c r="N56" s="27"/>
-      <c r="O56" s="27"/>
-      <c r="P56" s="27"/>
-      <c r="Q56" s="27"/>
-      <c r="R56" s="27"/>
-      <c r="S56" s="28"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="17"/>
+      <c r="R56" s="17"/>
+      <c r="S56" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B54:S54"/>
-    <mergeCell ref="B55:S55"/>
-    <mergeCell ref="B56:S56"/>
-    <mergeCell ref="J48:S48"/>
-    <mergeCell ref="A50:S50"/>
-    <mergeCell ref="B51:S51"/>
-    <mergeCell ref="B52:S52"/>
-    <mergeCell ref="B53:S53"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="J47:S47"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="J22:S22"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="J18:S18"/>
+    <mergeCell ref="J19:S19"/>
+    <mergeCell ref="J20:S20"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J24:S24"/>
+    <mergeCell ref="J25:S25"/>
+    <mergeCell ref="J26:S26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J27:S27"/>
+    <mergeCell ref="J28:S28"/>
+    <mergeCell ref="J29:S29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="J30:S30"/>
+    <mergeCell ref="J31:S31"/>
+    <mergeCell ref="J32:S32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="J34:S34"/>
+    <mergeCell ref="J35:S35"/>
     <mergeCell ref="J45:S45"/>
     <mergeCell ref="J46:S46"/>
     <mergeCell ref="B45:H45"/>
@@ -3317,48 +3341,24 @@
     <mergeCell ref="J42:S42"/>
     <mergeCell ref="J43:S43"/>
     <mergeCell ref="J44:S44"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="J34:S34"/>
-    <mergeCell ref="J35:S35"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="J30:S30"/>
-    <mergeCell ref="J31:S31"/>
-    <mergeCell ref="J32:S32"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J27:S27"/>
-    <mergeCell ref="J28:S28"/>
-    <mergeCell ref="J29:S29"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="J24:S24"/>
-    <mergeCell ref="J25:S25"/>
-    <mergeCell ref="J26:S26"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="J18:S18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="J20:S20"/>
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="A1:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B54:S54"/>
+    <mergeCell ref="B55:S55"/>
+    <mergeCell ref="B56:S56"/>
+    <mergeCell ref="J48:S48"/>
+    <mergeCell ref="A50:S50"/>
+    <mergeCell ref="B51:S51"/>
+    <mergeCell ref="B52:S52"/>
+    <mergeCell ref="B53:S53"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="J47:S47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3366,12 +3366,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7005DF65C69D244A0053930B4D80895" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfe4224a46d45a1569ee43293fdcdd48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a217f1db-afc0-486b-a03f-32483c6d35f7" xmlns:ns4="b3fc9c33-149f-45e5-9bdb-a4f7fe310215" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d8dd93a9b58d240e8e3304885c0c0fa" ns3:_="" ns4:_="">
     <xsd:import namespace="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
@@ -3588,6 +3582,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3598,23 +3598,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D0DA503-506E-48B5-9538-4DAB746C5D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3633,6 +3616,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916385B-7771-4B86-AC30-95BD0DD5FA1F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Implemented ablility to generate reports from GUI
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF788C8-5D02-428B-9769-851E26327387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5A631E-8F90-458D-B5D9-273189AE7BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
@@ -535,27 +535,6 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* koji se podaci nalaze u izvještaju
-* sadrži li izvještaj podatke iz tablica koje su u odnosu master-detail, te koje su to tablice
-* u kojim je formatima moguće spremiti izvještaj</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>* koji su sve jezici podržani</t>
     </r>
     <r>
@@ -1152,6 +1131,72 @@
       </rPr>
       <t>4. Forma za prikaz slike iz baze podataka (show_image_form.py)
 Ova forma sluzi za prikaz binarnog podatka (slike) iz baze podatka</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* koji se podaci nalaze u izvještaju
+* sadrži li izvještaj podatke iz tablica koje su u odnosu master-detail, te koje su to tablice
+* u kojim je formatima moguće spremiti izvještaj</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija komentar:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Aplikacija prikazuje generira dva izvjesaja. Klikom na button "Show reports" otvara se nova forma koja sadrzi dva TextBrowser widgeta koji prikazuju izvjestaje
+1. </t>
     </r>
   </si>
 </sst>
@@ -1492,10 +1537,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1520,36 +1595,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1868,8 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:H28"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28:S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,1451 +1925,1427 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
+      <c r="A7" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="31"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
     </row>
     <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="32"/>
-      <c r="S17" s="32"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
     </row>
     <row r="18" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="28" t="s">
+      <c r="J18" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
     </row>
     <row r="19" spans="1:20" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
     </row>
     <row r="20" spans="1:20" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
+      <c r="J20" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
       <c r="T20" s="12"/>
     </row>
     <row r="21" spans="1:20" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>3</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
+      <c r="J21" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
     </row>
     <row r="22" spans="1:20" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>4</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="B22" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
+      <c r="J22" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
     </row>
     <row r="23" spans="1:20" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="B23" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
+      <c r="J23" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
     </row>
     <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>6</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
+      <c r="J24" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
     </row>
     <row r="25" spans="1:20" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>7</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="26"/>
+      <c r="J25" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="24"/>
     </row>
     <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>8</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
+      <c r="J26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
     </row>
     <row r="27" spans="1:20" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>9</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
+      <c r="J27" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
     </row>
     <row r="28" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>10</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="B28" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
+      <c r="J28" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
     </row>
     <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>11</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="B29" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
+      <c r="J29" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
     </row>
     <row r="30" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>12</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="14" t="s">
+      <c r="J30" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
     </row>
     <row r="31" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="B31" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="14" t="s">
+      <c r="J31" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
     </row>
     <row r="32" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>14</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="14" t="s">
+      <c r="J32" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
+      <c r="B33" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="J33" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
+      <c r="B34" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="14" t="s">
+      <c r="J34" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>17</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="14" t="s">
+      <c r="J35" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>18</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="14" t="s">
+      <c r="J36" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="14"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
+      <c r="B37" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="14" t="s">
+      <c r="J37" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
     </row>
     <row r="38" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>20</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="14" t="s">
+      <c r="J38" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="18"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
-      <c r="B39" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
+      <c r="B39" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="14"/>
-      <c r="Q39" s="14"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="14"/>
+      <c r="J39" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>22</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="14" t="s">
+      <c r="J40" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="14"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="14"/>
+      <c r="J41" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
+      <c r="J42" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="18"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
+      <c r="B43" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
+      <c r="J43" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="14" t="s">
+      <c r="J44" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="14" t="s">
+      <c r="J45" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="14"/>
-      <c r="P45" s="14"/>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="14" t="s">
+      <c r="J46" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="14"/>
-      <c r="P46" s="14"/>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="14"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18"/>
+      <c r="S46" s="18"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="14" t="s">
+      <c r="J47" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
-      <c r="O47" s="14"/>
-      <c r="P47" s="14"/>
-      <c r="Q47" s="14"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="14"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="14" t="s">
+      <c r="J48" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-      <c r="Q48" s="14"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="14"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="18"/>
+      <c r="S48" s="18"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
-      <c r="K50" s="19"/>
-      <c r="L50" s="19"/>
-      <c r="M50" s="19"/>
-      <c r="N50" s="19"/>
-      <c r="O50" s="19"/>
-      <c r="P50" s="19"/>
-      <c r="Q50" s="19"/>
-      <c r="R50" s="19"/>
-      <c r="S50" s="19"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="29"/>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="29"/>
+      <c r="Q50" s="29"/>
+      <c r="R50" s="29"/>
+      <c r="S50" s="29"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
-      <c r="N51" s="20"/>
-      <c r="O51" s="20"/>
-      <c r="P51" s="20"/>
-      <c r="Q51" s="20"/>
-      <c r="R51" s="20"/>
-      <c r="S51" s="21"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="30"/>
+      <c r="L51" s="30"/>
+      <c r="M51" s="30"/>
+      <c r="N51" s="30"/>
+      <c r="O51" s="30"/>
+      <c r="P51" s="30"/>
+      <c r="Q51" s="30"/>
+      <c r="R51" s="30"/>
+      <c r="S51" s="31"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-      <c r="K52" s="15"/>
-      <c r="L52" s="15"/>
-      <c r="M52" s="15"/>
-      <c r="N52" s="15"/>
-      <c r="O52" s="15"/>
-      <c r="P52" s="15"/>
-      <c r="Q52" s="15"/>
-      <c r="R52" s="15"/>
-      <c r="S52" s="16"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="25"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="25"/>
+      <c r="N52" s="25"/>
+      <c r="O52" s="25"/>
+      <c r="P52" s="25"/>
+      <c r="Q52" s="25"/>
+      <c r="R52" s="25"/>
+      <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
-      <c r="P53" s="15"/>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="15"/>
-      <c r="S53" s="16"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="25"/>
+      <c r="O53" s="25"/>
+      <c r="P53" s="25"/>
+      <c r="Q53" s="25"/>
+      <c r="R53" s="25"/>
+      <c r="S53" s="26"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="15"/>
-      <c r="M54" s="15"/>
-      <c r="N54" s="15"/>
-      <c r="O54" s="15"/>
-      <c r="P54" s="15"/>
-      <c r="Q54" s="15"/>
-      <c r="R54" s="15"/>
-      <c r="S54" s="16"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="25"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="25"/>
+      <c r="N54" s="25"/>
+      <c r="O54" s="25"/>
+      <c r="P54" s="25"/>
+      <c r="Q54" s="25"/>
+      <c r="R54" s="25"/>
+      <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="15"/>
-      <c r="M55" s="15"/>
-      <c r="N55" s="15"/>
-      <c r="O55" s="15"/>
-      <c r="P55" s="15"/>
-      <c r="Q55" s="15"/>
-      <c r="R55" s="15"/>
-      <c r="S55" s="16"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="25"/>
+      <c r="K55" s="25"/>
+      <c r="L55" s="25"/>
+      <c r="M55" s="25"/>
+      <c r="N55" s="25"/>
+      <c r="O55" s="25"/>
+      <c r="P55" s="25"/>
+      <c r="Q55" s="25"/>
+      <c r="R55" s="25"/>
+      <c r="S55" s="26"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
-      <c r="J56" s="17"/>
-      <c r="K56" s="17"/>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="17"/>
-      <c r="O56" s="17"/>
-      <c r="P56" s="17"/>
-      <c r="Q56" s="17"/>
-      <c r="R56" s="17"/>
-      <c r="S56" s="18"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="27"/>
+      <c r="J56" s="27"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="27"/>
+      <c r="M56" s="27"/>
+      <c r="N56" s="27"/>
+      <c r="O56" s="27"/>
+      <c r="P56" s="27"/>
+      <c r="Q56" s="27"/>
+      <c r="R56" s="27"/>
+      <c r="S56" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="A1:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A16:S17"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="J18:S18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="J20:S20"/>
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="J24:S24"/>
-    <mergeCell ref="J25:S25"/>
-    <mergeCell ref="J26:S26"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J27:S27"/>
-    <mergeCell ref="J28:S28"/>
-    <mergeCell ref="J29:S29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="J30:S30"/>
-    <mergeCell ref="J31:S31"/>
-    <mergeCell ref="J32:S32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="J34:S34"/>
-    <mergeCell ref="J35:S35"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B54:S54"/>
+    <mergeCell ref="B55:S55"/>
+    <mergeCell ref="B56:S56"/>
+    <mergeCell ref="J48:S48"/>
+    <mergeCell ref="A50:S50"/>
+    <mergeCell ref="B51:S51"/>
+    <mergeCell ref="B52:S52"/>
+    <mergeCell ref="B53:S53"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="J47:S47"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
     <mergeCell ref="J45:S45"/>
     <mergeCell ref="J46:S46"/>
     <mergeCell ref="B45:H45"/>
@@ -3341,24 +3362,48 @@
     <mergeCell ref="J42:S42"/>
     <mergeCell ref="J43:S43"/>
     <mergeCell ref="J44:S44"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B54:S54"/>
-    <mergeCell ref="B55:S55"/>
-    <mergeCell ref="B56:S56"/>
-    <mergeCell ref="J48:S48"/>
-    <mergeCell ref="A50:S50"/>
-    <mergeCell ref="B51:S51"/>
-    <mergeCell ref="B52:S52"/>
-    <mergeCell ref="B53:S53"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="J47:S47"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="J34:S34"/>
+    <mergeCell ref="J35:S35"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="J30:S30"/>
+    <mergeCell ref="J31:S31"/>
+    <mergeCell ref="J32:S32"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J27:S27"/>
+    <mergeCell ref="J28:S28"/>
+    <mergeCell ref="J29:S29"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J24:S24"/>
+    <mergeCell ref="J25:S25"/>
+    <mergeCell ref="J26:S26"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="J22:S22"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="J18:S18"/>
+    <mergeCell ref="J19:S19"/>
+    <mergeCell ref="J20:S20"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A16:S17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3366,6 +3411,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7005DF65C69D244A0053930B4D80895" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfe4224a46d45a1569ee43293fdcdd48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a217f1db-afc0-486b-a03f-32483c6d35f7" xmlns:ns4="b3fc9c33-149f-45e5-9bdb-a4f7fe310215" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d8dd93a9b58d240e8e3304885c0c0fa" ns3:_="" ns4:_="">
     <xsd:import namespace="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
@@ -3582,12 +3633,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3598,6 +3643,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D0DA503-506E-48B5-9538-4DAB746C5D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3616,23 +3678,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916385B-7771-4B86-AC30-95BD0DD5FA1F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fully implemented ability to generate reports
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5A631E-8F90-458D-B5D9-273189AE7BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5D6DB1-7484-43C5-94B0-6C57FEB7D11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -1195,8 +1195,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Aplikacija prikazuje generira dva izvjesaja. Klikom na button "Show reports" otvara se nova forma koja sadrzi dva TextBrowser widgeta koji prikazuju izvjestaje
-1. </t>
+      <t>Aplikacija prikazuje generira dva izvjesaja. Klikom na button "Show reports" otvara se nova forma koja sadrzi dva TextBrowser widgeta koji prikazuju izvjestaje:
+1. Izvjestaj iz tablice proizvodi
+Sadrzaj:
+- opis iz koje tablice je izvjesataj
+- datum generiranja izvjesaja
+- naziv svakog proizvoda iz tablice, negova kategorija, cijena, kolicina i id skladista kojem pripada
+- ukupan iznos svih proizvoda, koluko je ukupno stavki u tablici , te ukupna kolicina svih proizvoda (zbroj kolicina svih proizvoda)
+2. Izvjestaj iz master-detal relacije, tablice skladista-proizvodi
+Ispod gumba "Show reports" se nalazi gumb "Generate reports" koji na click generira dva reporta i sprema ih u folder "reports".
+1. RTF izvjestaj o tablicama proizvodi
+2. PDF izvjestaj o master-detail relaciji, tablica skladista-proizvodi</t>
     </r>
   </si>
 </sst>
@@ -1537,40 +1546,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1595,6 +1574,36 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1925,1427 +1934,1451 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
     </row>
     <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
     </row>
     <row r="18" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="20" t="s">
+      <c r="J18" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
     </row>
     <row r="19" spans="1:20" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="18" t="s">
+      <c r="J19" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
     </row>
     <row r="20" spans="1:20" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="J20" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
       <c r="T20" s="12"/>
     </row>
     <row r="21" spans="1:20" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>3</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="18" t="s">
+      <c r="J21" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
     </row>
     <row r="22" spans="1:20" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>4</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="18" t="s">
+      <c r="J22" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
     </row>
     <row r="23" spans="1:20" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="18" t="s">
+      <c r="J23" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
     </row>
     <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>6</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="18" t="s">
+      <c r="J24" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
     </row>
     <row r="25" spans="1:20" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>7</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="22" t="s">
+      <c r="J25" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="24"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>8</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="18" t="s">
+      <c r="J26" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
     </row>
     <row r="27" spans="1:20" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>9</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="18" t="s">
+      <c r="J27" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
     </row>
     <row r="28" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="A28" s="10">
         <v>10</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="18" t="s">
+      <c r="J28" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
     </row>
     <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>11</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="18" t="s">
+      <c r="J29" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="21"/>
-      <c r="S29" s="21"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
     </row>
     <row r="30" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>12</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="18" t="s">
+      <c r="J30" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
     </row>
     <row r="31" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="18" t="s">
+      <c r="J31" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
     </row>
     <row r="32" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>14</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="18" t="s">
+      <c r="J32" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="18" t="s">
+      <c r="J33" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="18" t="s">
+      <c r="J34" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>17</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="18" t="s">
+      <c r="J35" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>18</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="18" t="s">
+      <c r="J36" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="18"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="18" t="s">
+      <c r="J37" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
     </row>
     <row r="38" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>20</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="18" t="s">
+      <c r="J38" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="18" t="s">
+      <c r="J39" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>22</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="18" t="s">
+      <c r="J40" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="18" t="s">
+      <c r="J41" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="18" t="s">
+      <c r="J42" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="18" t="s">
+      <c r="J43" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="18" t="s">
+      <c r="J44" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="18" t="s">
+      <c r="J45" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="18" t="s">
+      <c r="J46" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="14"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="18" t="s">
+      <c r="J47" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="18" t="s">
+      <c r="J48" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="18"/>
-      <c r="O48" s="18"/>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="18"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
-      <c r="N50" s="29"/>
-      <c r="O50" s="29"/>
-      <c r="P50" s="29"/>
-      <c r="Q50" s="29"/>
-      <c r="R50" s="29"/>
-      <c r="S50" s="29"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="30"/>
-      <c r="M51" s="30"/>
-      <c r="N51" s="30"/>
-      <c r="O51" s="30"/>
-      <c r="P51" s="30"/>
-      <c r="Q51" s="30"/>
-      <c r="R51" s="30"/>
-      <c r="S51" s="31"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="20"/>
+      <c r="O51" s="20"/>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="20"/>
+      <c r="S51" s="21"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="25"/>
-      <c r="L52" s="25"/>
-      <c r="M52" s="25"/>
-      <c r="N52" s="25"/>
-      <c r="O52" s="25"/>
-      <c r="P52" s="25"/>
-      <c r="Q52" s="25"/>
-      <c r="R52" s="25"/>
-      <c r="S52" s="26"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="15"/>
+      <c r="O52" s="15"/>
+      <c r="P52" s="15"/>
+      <c r="Q52" s="15"/>
+      <c r="R52" s="15"/>
+      <c r="S52" s="16"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
-      <c r="O53" s="25"/>
-      <c r="P53" s="25"/>
-      <c r="Q53" s="25"/>
-      <c r="R53" s="25"/>
-      <c r="S53" s="26"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="15"/>
+      <c r="S53" s="16"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
-      <c r="L54" s="25"/>
-      <c r="M54" s="25"/>
-      <c r="N54" s="25"/>
-      <c r="O54" s="25"/>
-      <c r="P54" s="25"/>
-      <c r="Q54" s="25"/>
-      <c r="R54" s="25"/>
-      <c r="S54" s="26"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+      <c r="S54" s="16"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="25"/>
-      <c r="L55" s="25"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="25"/>
-      <c r="O55" s="25"/>
-      <c r="P55" s="25"/>
-      <c r="Q55" s="25"/>
-      <c r="R55" s="25"/>
-      <c r="S55" s="26"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="15"/>
+      <c r="R55" s="15"/>
+      <c r="S55" s="16"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="27"/>
-      <c r="J56" s="27"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="27"/>
-      <c r="N56" s="27"/>
-      <c r="O56" s="27"/>
-      <c r="P56" s="27"/>
-      <c r="Q56" s="27"/>
-      <c r="R56" s="27"/>
-      <c r="S56" s="28"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="17"/>
+      <c r="R56" s="17"/>
+      <c r="S56" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B54:S54"/>
-    <mergeCell ref="B55:S55"/>
-    <mergeCell ref="B56:S56"/>
-    <mergeCell ref="J48:S48"/>
-    <mergeCell ref="A50:S50"/>
-    <mergeCell ref="B51:S51"/>
-    <mergeCell ref="B52:S52"/>
-    <mergeCell ref="B53:S53"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="J47:S47"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="J22:S22"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="J18:S18"/>
+    <mergeCell ref="J19:S19"/>
+    <mergeCell ref="J20:S20"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J24:S24"/>
+    <mergeCell ref="J25:S25"/>
+    <mergeCell ref="J26:S26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J27:S27"/>
+    <mergeCell ref="J28:S28"/>
+    <mergeCell ref="J29:S29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="J30:S30"/>
+    <mergeCell ref="J31:S31"/>
+    <mergeCell ref="J32:S32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="J34:S34"/>
+    <mergeCell ref="J35:S35"/>
     <mergeCell ref="J45:S45"/>
     <mergeCell ref="J46:S46"/>
     <mergeCell ref="B45:H45"/>
@@ -3362,48 +3395,24 @@
     <mergeCell ref="J42:S42"/>
     <mergeCell ref="J43:S43"/>
     <mergeCell ref="J44:S44"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="J34:S34"/>
-    <mergeCell ref="J35:S35"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="J30:S30"/>
-    <mergeCell ref="J31:S31"/>
-    <mergeCell ref="J32:S32"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J27:S27"/>
-    <mergeCell ref="J28:S28"/>
-    <mergeCell ref="J29:S29"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="J24:S24"/>
-    <mergeCell ref="J25:S25"/>
-    <mergeCell ref="J26:S26"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="J18:S18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="J20:S20"/>
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="A1:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B54:S54"/>
+    <mergeCell ref="B55:S55"/>
+    <mergeCell ref="B56:S56"/>
+    <mergeCell ref="J48:S48"/>
+    <mergeCell ref="A50:S50"/>
+    <mergeCell ref="B51:S51"/>
+    <mergeCell ref="B52:S52"/>
+    <mergeCell ref="B53:S53"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="J47:S47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3411,12 +3420,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7005DF65C69D244A0053930B4D80895" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfe4224a46d45a1569ee43293fdcdd48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a217f1db-afc0-486b-a03f-32483c6d35f7" xmlns:ns4="b3fc9c33-149f-45e5-9bdb-a4f7fe310215" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d8dd93a9b58d240e8e3304885c0c0fa" ns3:_="" ns4:_="">
     <xsd:import namespace="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
@@ -3633,6 +3636,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3643,23 +3652,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D0DA503-506E-48B5-9538-4DAB746C5D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3678,6 +3670,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916385B-7771-4B86-AC30-95BD0DD5FA1F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Implemented multithreading on generate and save reports
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5D6DB1-7484-43C5-94B0-6C57FEB7D11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC79AB8-3189-4C63-9A2D-8484B988B437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
@@ -276,50 +276,6 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">* nazive klasa, atributa i metoda (ukoliko projekt sadrži mnogo klasa/atributa/metoda dovoljno je navesti samo 3 klase s po minimalno 2 atributa i metode)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Napomena: priznaju se samo klase koje je student napisao (ne priznaju se automatski generirane klase od strane razvojnog okruženja/programskog jezika).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>* koji se podaci prenose u mrežnoj komunikaciji (što šalje klijent, a što vraća poslužitelj)
 * razmjenjuju li se osim jednostavnih tipova podataka u komunikaciji i tokovi podataka (eng. streams), te što se u njima nalazi</t>
     </r>
@@ -683,40 +639,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">* korištenu strukturu podataka (npr. Student koji ima ime, prezime, jmbag itd.)
-* podržane operacije nad prethodno opisanom strukturom podataka (čitanje i/ili pisanje)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Napomena 1: u datotekama treba upravljati nizovima zapisa, ne samo jednim zapisom
-Napomena 2: korištena struktura podataka ne može biti ista kao i u slučaju XML/JSON funkcionalnosti (i obrnuto).</t>
-    </r>
-  </si>
-  <si>
     <t>Za spremanje i obradu podataka u aplikaciji demonstrirati korištenje XML ili JSON tipa datoteka. Potrebno je demonstrirati operacije čitanja, pisanja, uređivanja i brisanja podataka. (3 boda) U slučaju da aplikacija koristi oba pristupa (XML + JSON) moguće je dobiti 6 bodova.</t>
   </si>
   <si>
@@ -727,63 +649,6 @@
   </si>
   <si>
     <t>Aplikacija demonstrira korištenje barem jednog mehanizma međusobnog zaključavanja (npr. kritična sekcija ili mutex), 2 boda. U slučaju da se koriste dva različita mehanizma međusobnog zaključavanja moguće je dobiti 4 boda.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* koje se operacije izvršavaju paralelno, tj. korištenjem više dretvi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">* da li se koristi bazen dretvi 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Napomena: priznat će se samo operacije gdje upotreba više dretvi (paralelno izvršavanje koda) daje bolje performanse u radu aplikacije u odnosu na izvršavanje tih istih operacija korištenjem samo jedne dretve.</t>
-    </r>
   </si>
   <si>
     <t>Demonstrirati UDP klijent-poslužitelj komunikaciju u kojoj su klijent i poslužitelj implementirani u različitim aplikacijama. Potrebno je prikazati primjer u kojemu se kao zahtjev/odgovor prenose jednostavni tipovi podataka (3 boda). U slučaju i prijenosa tokova (eng. streams) moguće je dobiti 5 bodova.</t>
@@ -1203,9 +1068,183 @@
 - naziv svakog proizvoda iz tablice, negova kategorija, cijena, kolicina i id skladista kojem pripada
 - ukupan iznos svih proizvoda, koluko je ukupno stavki u tablici , te ukupna kolicina svih proizvoda (zbroj kolicina svih proizvoda)
 2. Izvjestaj iz master-detal relacije, tablice skladista-proizvodi
-Ispod gumba "Show reports" se nalazi gumb "Generate reports" koji na click generira dva reporta i sprema ih u folder "reports".
+- opis iz koje tablice je izvjesataj
+- datum generiranja izvjesaja
+- ispis svakog skladista po ID-u te za svako skladiste proizvodi koji se u njemu nalaze. 
+  npr. skladiste 1 - proizvod 1 - atributi proizvoda 1
+                                  - proizvod 2 - atributi proizvoda 2
+           skladiste 2 - proizvod 1 - atributi proizvoda 1
+                                  - ...
+- nakon ispisa svakog proizvoda za pojedinacno skladiste se nalazi izvjestaj koliki je ukupni iznos proizvoda za pojedinacno skladiste, ukupno stavki u skladistu, te koliko je ukupno porizvoda u skladistu
+- na kraju dokumenta je zbroj svih podataka za sva skladista kao u prethodnom izvjestaju
+Ispod gumba "Show reports" se nalazi gumb "Generate reports" koji na click generira dva reporta i sprema ih u folder "reports". Jedan report je u PDF formatu, a drugi u RTF formatu.
 1. RTF izvjestaj o tablicama proizvodi
 2. PDF izvjestaj o master-detail relaciji, tablica skladista-proizvodi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* nazive klasa, atributa i metoda (ukoliko projekt sadrži mnogo klasa/atributa/metoda dovoljno je navesti samo 3 klase s po minimalno 2 atributa i metode)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Napomena: priznaju se samo klase koje je student napisao (ne priznaju se automatski generirane klase od strane razvojnog okruženja/programskog jezika).
+Matija</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* koje se operacije izvršavaju paralelno, tj. korištenjem više dretvi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* da li se koristi bazen dretvi 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Napomena: priznat će se samo operacije gdje upotreba više dretvi (paralelno izvršavanje koda) daje bolje performanse u radu aplikacije u odnosu na izvršavanje tih istih operacija korištenjem samo jedne dretve.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Matija komentar:
+Koristen python module concurrent.futures za Parrael task. Taj module omogucuje koristenje subclase ThreadPoolExecutor.
+Konstruktor klase  ParallelTaskExecutor kao argument prima koliko ce maksimalno dretvi/thredova biti dostupno u bazenu dretvi.
+Paralelno se izvadjaju tri funkcije za generiranje i spremanje izvjesataja.  Svaka funkcija 
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* korištenu strukturu podataka (npr. Student koji ima ime, prezime, jmbag itd.)
+* podržane operacije nad prethodno opisanom strukturom podataka (čitanje i/ili pisanje)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Napomena 1: u datotekama treba upravljati nizovima zapisa, ne samo jednim zapisom
+Napomena 2: korištena struktura podataka ne može biti ista kao i u slučaju XML/JSON funkcionalnosti (i obrnuto).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija komentar:
+U aplikaciji se koristi binarni zapis slike koji se naknadno kroz GUI aplikacije sprema u bazu podataka.
+U tablici proizvodi, slika proizvoda se sprema u polje "privitak" u MS Access binarni tip podataka "Long binary data".  Kada se slika ucita pomocu file systema, pretvori u binarni zapis te se takva zapise u bazu podataka.
+Slika se u GUI aplikacije moze prikazati pomocu gumba "Show picture" u tabu "Add/Show product picutre"</t>
     </r>
   </si>
 </sst>
@@ -1922,8 +1961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28:S28"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24:S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2049,7 +2088,7 @@
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B7" s="31"/>
       <c r="C7" s="31"/>
@@ -2309,7 +2348,7 @@
         <v>3</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="K19" s="23"/>
       <c r="L19" s="23"/>
@@ -2338,7 +2377,7 @@
         <v>3</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
@@ -2368,7 +2407,7 @@
         <v>4</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
@@ -2385,7 +2424,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -2397,7 +2436,7 @@
         <v>4</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
@@ -2414,7 +2453,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -2426,7 +2465,7 @@
         <v>6</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
@@ -2439,7 +2478,7 @@
       <c r="S23" s="14"/>
     </row>
     <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="A24" s="10">
         <v>6</v>
       </c>
       <c r="B24" s="13" t="s">
@@ -2455,7 +2494,7 @@
         <v>3</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
@@ -2484,7 +2523,7 @@
         <v>5</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K25" s="25"/>
       <c r="L25" s="25"/>
@@ -2513,7 +2552,7 @@
         <v>4</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
@@ -2542,7 +2581,7 @@
         <v>3</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K27" s="14"/>
       <c r="L27" s="14"/>
@@ -2559,7 +2598,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -2571,7 +2610,7 @@
         <v>4</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
@@ -2584,11 +2623,11 @@
       <c r="S28" s="14"/>
     </row>
     <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+      <c r="A29" s="10">
         <v>11</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -2600,7 +2639,7 @@
         <v>5</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="K29" s="23"/>
       <c r="L29" s="23"/>
@@ -2646,7 +2685,7 @@
         <v>13</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -2704,7 +2743,7 @@
         <v>15</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -2716,7 +2755,7 @@
         <v>5</v>
       </c>
       <c r="J33" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K33" s="14"/>
       <c r="L33" s="14"/>
@@ -2733,7 +2772,7 @@
         <v>16</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -2745,7 +2784,7 @@
         <v>5</v>
       </c>
       <c r="J34" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K34" s="14"/>
       <c r="L34" s="14"/>
@@ -2774,7 +2813,7 @@
         <v>3</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K35" s="14"/>
       <c r="L35" s="14"/>
@@ -2803,7 +2842,7 @@
         <v>3</v>
       </c>
       <c r="J36" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K36" s="14"/>
       <c r="L36" s="14"/>
@@ -2820,7 +2859,7 @@
         <v>19</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
@@ -2832,7 +2871,7 @@
         <v>6</v>
       </c>
       <c r="J37" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K37" s="14"/>
       <c r="L37" s="14"/>
@@ -2861,7 +2900,7 @@
         <v>3</v>
       </c>
       <c r="J38" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K38" s="14"/>
       <c r="L38" s="14"/>
@@ -2878,7 +2917,7 @@
         <v>21</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
@@ -2890,7 +2929,7 @@
         <v>6</v>
       </c>
       <c r="J39" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K39" s="14"/>
       <c r="L39" s="14"/>
@@ -2919,7 +2958,7 @@
         <v>4</v>
       </c>
       <c r="J40" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K40" s="14"/>
       <c r="L40" s="14"/>
@@ -2948,7 +2987,7 @@
         <v>2</v>
       </c>
       <c r="J41" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K41" s="14"/>
       <c r="L41" s="14"/>
@@ -2977,7 +3016,7 @@
         <v>3</v>
       </c>
       <c r="J42" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K42" s="14"/>
       <c r="L42" s="14"/>
@@ -2994,7 +3033,7 @@
         <v>25</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
@@ -3006,7 +3045,7 @@
         <v>7</v>
       </c>
       <c r="J43" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K43" s="14"/>
       <c r="L43" s="14"/>
@@ -3035,7 +3074,7 @@
         <v>4</v>
       </c>
       <c r="J44" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K44" s="14"/>
       <c r="L44" s="14"/>
@@ -3064,7 +3103,7 @@
         <v>3</v>
       </c>
       <c r="J45" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K45" s="14"/>
       <c r="L45" s="14"/>
@@ -3093,7 +3132,7 @@
         <v>3</v>
       </c>
       <c r="J46" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K46" s="14"/>
       <c r="L46" s="14"/>
@@ -3122,7 +3161,7 @@
         <v>3</v>
       </c>
       <c r="J47" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K47" s="14"/>
       <c r="L47" s="14"/>
@@ -3151,7 +3190,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K48" s="14"/>
       <c r="L48" s="14"/>

</xml_diff>

<commit_message>
When you would lookup products by warehouse ID (button 'Select warehouse'), at column 'privitak' user would get binary characters instead if attachment is in the database or not. That would couse lags becouse of the length of the binary character. Instead of that, not shows 'Available' or 'N/A'
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC79AB8-3189-4C63-9A2D-8484B988B437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC9EF25-200D-4C57-8244-152FA28A3055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
@@ -1961,8 +1961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24:S24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented ability to refresh GUI information using QThreads
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC9EF25-200D-4C57-8244-152FA28A3055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F33AB75-4649-49DE-ABCB-8B0B36399592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
@@ -257,25 +257,6 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* što se u korisničkom sučelju ažurira iz dretve</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>* koji se podaci prenose u mrežnoj komunikaciji (što šalje klijent, a što vraća poslužitelj)
 * razmjenjuju li se osim jednostavnih tipova podataka u komunikaciji i tokovi podataka (eng. streams), te što se u njima nalazi</t>
     </r>
@@ -1247,12 +1228,46 @@
 Slika se u GUI aplikacije moze prikazati pomocu gumba "Show picture" u tabu "Add/Show product picutre"</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* što se u korisničkom sučelju ažurira iz dretve
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Matija komentar:
+U MS Access bazi podataka skladiste, tablica proizvodi, stupac privitak sadrži binarny sadržaj tipa OLE Object, tj. binarno zapisana slika proizvoda.
+U aplikaciji se po proizvod_id moze dodati tabu 'Add/Show product picture' moze dodati i prikazati slika iz base podataka.
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1334,6 +1349,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color rgb="FF002060"/>
       <name val="Calibri"/>
@@ -1585,10 +1608,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1613,36 +1666,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1961,8 +1984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29:S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,1451 +1996,1427 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
+      <c r="A7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="31"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
     </row>
     <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="32"/>
-      <c r="S17" s="32"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
     </row>
     <row r="18" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="28" t="s">
+      <c r="J18" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
     </row>
     <row r="19" spans="1:20" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
+      <c r="J19" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
     </row>
     <row r="20" spans="1:20" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
+      <c r="J20" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
       <c r="T20" s="12"/>
     </row>
     <row r="21" spans="1:20" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>3</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
+      <c r="J21" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
     </row>
     <row r="22" spans="1:20" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>4</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="B22" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
+      <c r="J22" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
     </row>
     <row r="23" spans="1:20" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="B23" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
+      <c r="J23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
     </row>
     <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>6</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
+      <c r="J24" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
     </row>
     <row r="25" spans="1:20" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>7</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="26"/>
+      <c r="J25" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="24"/>
     </row>
     <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>8</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
+      <c r="J26" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
     </row>
     <row r="27" spans="1:20" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>9</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
+      <c r="J27" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
     </row>
     <row r="28" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>10</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="B28" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
+      <c r="J28" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
     </row>
     <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>11</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="B29" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
+      <c r="J29" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
     </row>
     <row r="30" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+      <c r="A30" s="10">
         <v>12</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
+      <c r="J30" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
     </row>
     <row r="31" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="B31" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="14" t="s">
+      <c r="J31" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
     </row>
     <row r="32" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>14</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="14" t="s">
+      <c r="J32" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
+      <c r="B33" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
+      <c r="J33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
+      <c r="B34" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
+      <c r="J34" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>17</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
+      <c r="J35" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>18</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="14"/>
+      <c r="J36" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
+      <c r="B37" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
+      <c r="J37" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
     </row>
     <row r="38" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>20</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
+      <c r="J38" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="18"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
-      <c r="B39" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
+      <c r="B39" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="14"/>
-      <c r="Q39" s="14"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="14"/>
+      <c r="J39" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>22</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
+      <c r="J40" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="14"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="14"/>
+      <c r="J41" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
+      <c r="J42" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="18"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
+      <c r="B43" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
+      <c r="J43" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
+      <c r="J44" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="14"/>
-      <c r="P45" s="14"/>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
+      <c r="J45" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="14"/>
-      <c r="P46" s="14"/>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="14"/>
+      <c r="J46" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18"/>
+      <c r="S46" s="18"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
-      <c r="O47" s="14"/>
-      <c r="P47" s="14"/>
-      <c r="Q47" s="14"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="14"/>
+      <c r="J47" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-      <c r="Q48" s="14"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="14"/>
+      <c r="J48" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="18"/>
+      <c r="S48" s="18"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
-      <c r="K50" s="19"/>
-      <c r="L50" s="19"/>
-      <c r="M50" s="19"/>
-      <c r="N50" s="19"/>
-      <c r="O50" s="19"/>
-      <c r="P50" s="19"/>
-      <c r="Q50" s="19"/>
-      <c r="R50" s="19"/>
-      <c r="S50" s="19"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="29"/>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="29"/>
+      <c r="Q50" s="29"/>
+      <c r="R50" s="29"/>
+      <c r="S50" s="29"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
-      <c r="N51" s="20"/>
-      <c r="O51" s="20"/>
-      <c r="P51" s="20"/>
-      <c r="Q51" s="20"/>
-      <c r="R51" s="20"/>
-      <c r="S51" s="21"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="30"/>
+      <c r="L51" s="30"/>
+      <c r="M51" s="30"/>
+      <c r="N51" s="30"/>
+      <c r="O51" s="30"/>
+      <c r="P51" s="30"/>
+      <c r="Q51" s="30"/>
+      <c r="R51" s="30"/>
+      <c r="S51" s="31"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-      <c r="K52" s="15"/>
-      <c r="L52" s="15"/>
-      <c r="M52" s="15"/>
-      <c r="N52" s="15"/>
-      <c r="O52" s="15"/>
-      <c r="P52" s="15"/>
-      <c r="Q52" s="15"/>
-      <c r="R52" s="15"/>
-      <c r="S52" s="16"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="25"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="25"/>
+      <c r="N52" s="25"/>
+      <c r="O52" s="25"/>
+      <c r="P52" s="25"/>
+      <c r="Q52" s="25"/>
+      <c r="R52" s="25"/>
+      <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
-      <c r="P53" s="15"/>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="15"/>
-      <c r="S53" s="16"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="25"/>
+      <c r="O53" s="25"/>
+      <c r="P53" s="25"/>
+      <c r="Q53" s="25"/>
+      <c r="R53" s="25"/>
+      <c r="S53" s="26"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="15"/>
-      <c r="M54" s="15"/>
-      <c r="N54" s="15"/>
-      <c r="O54" s="15"/>
-      <c r="P54" s="15"/>
-      <c r="Q54" s="15"/>
-      <c r="R54" s="15"/>
-      <c r="S54" s="16"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="25"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="25"/>
+      <c r="N54" s="25"/>
+      <c r="O54" s="25"/>
+      <c r="P54" s="25"/>
+      <c r="Q54" s="25"/>
+      <c r="R54" s="25"/>
+      <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="15"/>
-      <c r="M55" s="15"/>
-      <c r="N55" s="15"/>
-      <c r="O55" s="15"/>
-      <c r="P55" s="15"/>
-      <c r="Q55" s="15"/>
-      <c r="R55" s="15"/>
-      <c r="S55" s="16"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="25"/>
+      <c r="K55" s="25"/>
+      <c r="L55" s="25"/>
+      <c r="M55" s="25"/>
+      <c r="N55" s="25"/>
+      <c r="O55" s="25"/>
+      <c r="P55" s="25"/>
+      <c r="Q55" s="25"/>
+      <c r="R55" s="25"/>
+      <c r="S55" s="26"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
-      <c r="J56" s="17"/>
-      <c r="K56" s="17"/>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="17"/>
-      <c r="O56" s="17"/>
-      <c r="P56" s="17"/>
-      <c r="Q56" s="17"/>
-      <c r="R56" s="17"/>
-      <c r="S56" s="18"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="27"/>
+      <c r="J56" s="27"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="27"/>
+      <c r="M56" s="27"/>
+      <c r="N56" s="27"/>
+      <c r="O56" s="27"/>
+      <c r="P56" s="27"/>
+      <c r="Q56" s="27"/>
+      <c r="R56" s="27"/>
+      <c r="S56" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="A1:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A16:S17"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="J18:S18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="J20:S20"/>
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="J24:S24"/>
-    <mergeCell ref="J25:S25"/>
-    <mergeCell ref="J26:S26"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J27:S27"/>
-    <mergeCell ref="J28:S28"/>
-    <mergeCell ref="J29:S29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="J30:S30"/>
-    <mergeCell ref="J31:S31"/>
-    <mergeCell ref="J32:S32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="J34:S34"/>
-    <mergeCell ref="J35:S35"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B54:S54"/>
+    <mergeCell ref="B55:S55"/>
+    <mergeCell ref="B56:S56"/>
+    <mergeCell ref="J48:S48"/>
+    <mergeCell ref="A50:S50"/>
+    <mergeCell ref="B51:S51"/>
+    <mergeCell ref="B52:S52"/>
+    <mergeCell ref="B53:S53"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="J47:S47"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
     <mergeCell ref="J45:S45"/>
     <mergeCell ref="J46:S46"/>
     <mergeCell ref="B45:H45"/>
@@ -3434,24 +3433,48 @@
     <mergeCell ref="J42:S42"/>
     <mergeCell ref="J43:S43"/>
     <mergeCell ref="J44:S44"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B54:S54"/>
-    <mergeCell ref="B55:S55"/>
-    <mergeCell ref="B56:S56"/>
-    <mergeCell ref="J48:S48"/>
-    <mergeCell ref="A50:S50"/>
-    <mergeCell ref="B51:S51"/>
-    <mergeCell ref="B52:S52"/>
-    <mergeCell ref="B53:S53"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="J47:S47"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="J34:S34"/>
+    <mergeCell ref="J35:S35"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="J30:S30"/>
+    <mergeCell ref="J31:S31"/>
+    <mergeCell ref="J32:S32"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J27:S27"/>
+    <mergeCell ref="J28:S28"/>
+    <mergeCell ref="J29:S29"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J24:S24"/>
+    <mergeCell ref="J25:S25"/>
+    <mergeCell ref="J26:S26"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="J22:S22"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="J18:S18"/>
+    <mergeCell ref="J19:S19"/>
+    <mergeCell ref="J20:S20"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A16:S17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3459,6 +3482,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7005DF65C69D244A0053930B4D80895" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfe4224a46d45a1569ee43293fdcdd48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a217f1db-afc0-486b-a03f-32483c6d35f7" xmlns:ns4="b3fc9c33-149f-45e5-9bdb-a4f7fe310215" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d8dd93a9b58d240e8e3304885c0c0fa" ns3:_="" ns4:_="">
     <xsd:import namespace="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
@@ -3675,12 +3704,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3691,6 +3714,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D0DA503-506E-48B5-9538-4DAB746C5D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3709,23 +3749,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916385B-7771-4B86-AC30-95BD0DD5FA1F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixed some sorting bugs
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F33AB75-4649-49DE-ABCB-8B0B36399592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3212BE68-5C54-44A0-B1B4-5BBDCBFB46F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -316,7 +316,8 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* na koji se web servis spaja aplikacija (naziv i link), te koje njegove resurse koristi</t>
+      <t>* zašto se koristi digitalni potpis i što se njime potpisuje
+* u kojem se trenutku događa potpisivanje, a kada verifikacija digitalnog potpisa</t>
     </r>
   </si>
   <si>
@@ -335,8 +336,8 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* zašto se koristi digitalni potpis i što se njime potpisuje
-* u kojem se trenutku događa potpisivanje, a kada verifikacija digitalnog potpisa</t>
+      <t>* koje se funkcije/klase/metode nalaze u dinamičkoj biblioteci
+* u koju se svrhu koriste navedene funkcije/klase/metode</t>
     </r>
   </si>
   <si>
@@ -355,8 +356,7 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* koje se funkcije/klase/metode nalaze u dinamičkoj biblioteci
-* u koju se svrhu koriste navedene funkcije/klase/metode</t>
+      <t>* koji se dijalozi nalaze u dinamičkoj biblioteci, te u koju svrhu se koriste</t>
     </r>
   </si>
   <si>
@@ -375,7 +375,7 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* koji se dijalozi nalaze u dinamičkoj biblioteci, te u koju svrhu se koriste</t>
+      <t>* koji se resursi nalaze u dinamičkoj biblioteci, te u koju svrhu se koriste</t>
     </r>
   </si>
   <si>
@@ -394,7 +394,7 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* koji se resursi nalaze u dinamičkoj biblioteci, te u koju svrhu se koriste</t>
+      <t>* na koji se način provodi autentifikacija i autorizacija, te koje ovlasti ima svaki od korisnika</t>
     </r>
   </si>
   <si>
@@ -413,7 +413,8 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* na koji se način provodi autentifikacija i autorizacija, te koje ovlasti ima svaki od korisnika</t>
+      <t>* koje se funkcije/klase/metode nalaze u statičkoj biblioteci
+* u koju se svrhu koriste navedene funkcije/klase/metode</t>
     </r>
   </si>
   <si>
@@ -432,8 +433,8 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* koje se funkcije/klase/metode nalaze u statičkoj biblioteci
-* u koju se svrhu koriste navedene funkcije/klase/metode</t>
+      <t>* u koju se svrhu koristi web servis te koje su njegove metode
+* je li web servis smješten na web poslužitelju (IIS, Apache ili sl.) ili u zasebnoj (desktop) aplikaciji</t>
     </r>
   </si>
   <si>
@@ -452,13 +453,18 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* u koju se svrhu koristi web servis te koje su njegove metode
-* je li web servis smješten na web poslužitelju (IIS, Apache ili sl.) ili u zasebnoj (desktop) aplikaciji</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
+      <t>* koji su sve jezici podržani</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -472,18 +478,12 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* koji su sve jezici podržani</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+      <t>* koliko dijaloga je prevedeno</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
 </t>
     </r>
     <r>
@@ -497,25 +497,6 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* koliko dijaloga je prevedeno</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">* koji se podaci šifriraju i dešifriraju u aplikaciji
 </t>
     </r>
@@ -529,28 +510,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Napomena: lozinke se ne šifriraju!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* gdje (nad kojom tablicom/tablicama) je podržana operacija sortiranja
-* gdje (nad kojom tablicom/tablicama) je podržana operacija filtriranja
-* gdje se koristi izračunato (eng. calculated) polje i što ono izračunava
-* gdje se koristi lookup polje (na što referencira i koju vrijednost ima)</t>
     </r>
   </si>
   <si>
@@ -1244,6 +1203,164 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
+      <t>* gdje (nad kojom tablicom/tablicama) je podržana operacija sortiranja
+* gdje (nad kojom tablicom/tablicama) je podržana operacija filtriranja
+* gdje se koristi izračunato (eng. calculated) polje i što ono izračunava
+* gdje se koristi lookup polje (na što referencira i koju vrijednost ima)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Matija komentar:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* gdje (nad kojom tablicom/tablicama) je podržana operacija sortiranja:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Opcija sortiranja je podrzana nad tablicom "proizvodi", "skladiste" (tablice se prikazuju klikom na gumbe "Show Products" i "Show warehouses")i tablici koja se filtrira po proizvodu te na lookup tablici. Sortiranje se obavlja tako da se klikne na header tablice, te ovisno o trenutnom redosljedu, sortira se suprutno (padajuce i rastuce sortiranje)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* gdje (nad kojom tablicom/tablicama) je podržana operacija filtriranja:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Operacija filtriranja je podrzana nad lookup opcijom. Skladista se mogu pretrazivati pomocu proizvoda koji se nalazi u njima. Koristiku se ispisuju sva skladista koja sadrze trazeni proizvod. Kada se u polje pored gumba "Find" unese kljucna rijec proizvoda, u widgetu za prikaz tablica se ispisuje tablica skladiste, proizvodi te njigovi atributi. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* gdje se koristi izračunato (eng. calculated) polje i što ono izračunava:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Opcija calculated field se koristi nad tablicom proizvodi. Ono izracunava kolika je ukupna cifra svih proizvoda koji se nalaze u tabili proizvodi (kolicina * cijena svih proizvoda)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* gdje se koristi lookup polje (na što referencira i koju vrijednost ima)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Lookup se koristi nad tablicom skladista i proizvodi. Kada se u polje iznad gumba "Select warehouse" unese ID skladista (nalazi se u grupboxu pod nazivom Selected warehouse information) u widgetu za prikaz koji se nalazi ispod ispisuje se tablica sa trazenim atributima skaldista te svaki proizvod i njegovi atributi koji pripradaju tom skladistu. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">* što se u korisničkom sučelju ažurira iz dretve
 </t>
     </r>
@@ -1257,9 +1374,40 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Matija komentar:
-U MS Access bazi podataka skladiste, tablica proizvodi, stupac privitak sadrži binarny sadržaj tipa OLE Object, tj. binarno zapisana slika proizvoda.
-U aplikaciji se po proizvod_id moze dodati tabu 'Add/Show product picture' moze dodati i prikazati slika iz base podataka.
-</t>
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* na koji se web servis spaja aplikacija (naziv i link), te koje njegove resurse koristi
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija komentar:
+Aplikacija se sapaja na freecurrencyapi, sa kojega dohvaca trenutnu vrijednost tecaja
+https://freecurrencyapi.com/
+https://github.com/everapihq/freecurrencyapi-python</t>
     </r>
   </si>
 </sst>
@@ -1267,7 +1415,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1357,6 +1505,14 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF002060"/>
       <name val="Calibri"/>
@@ -1984,8 +2140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29:S29"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2111,7 +2267,7 @@
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -2371,7 +2527,7 @@
         <v>3</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K19" s="21"/>
       <c r="L19" s="21"/>
@@ -2400,7 +2556,7 @@
         <v>3</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K20" s="18"/>
       <c r="L20" s="18"/>
@@ -2430,7 +2586,7 @@
         <v>4</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K21" s="18"/>
       <c r="L21" s="18"/>
@@ -2447,7 +2603,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -2459,7 +2615,7 @@
         <v>4</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
@@ -2476,7 +2632,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
@@ -2488,7 +2644,7 @@
         <v>6</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K23" s="18"/>
       <c r="L23" s="18"/>
@@ -2517,7 +2673,7 @@
         <v>3</v>
       </c>
       <c r="J24" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K24" s="18"/>
       <c r="L24" s="18"/>
@@ -2546,7 +2702,7 @@
         <v>5</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K25" s="23"/>
       <c r="L25" s="23"/>
@@ -2559,7 +2715,7 @@
       <c r="S25" s="24"/>
     </row>
     <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="10">
         <v>8</v>
       </c>
       <c r="B26" s="16" t="s">
@@ -2575,7 +2731,7 @@
         <v>4</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="K26" s="18"/>
       <c r="L26" s="18"/>
@@ -2604,7 +2760,7 @@
         <v>3</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K27" s="18"/>
       <c r="L27" s="18"/>
@@ -2621,7 +2777,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -2633,7 +2789,7 @@
         <v>4</v>
       </c>
       <c r="J28" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K28" s="18"/>
       <c r="L28" s="18"/>
@@ -2650,7 +2806,7 @@
         <v>11</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
@@ -2662,7 +2818,7 @@
         <v>5</v>
       </c>
       <c r="J29" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K29" s="21"/>
       <c r="L29" s="21"/>
@@ -2691,7 +2847,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K30" s="18"/>
       <c r="L30" s="18"/>
@@ -2708,7 +2864,7 @@
         <v>13</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -2766,7 +2922,7 @@
         <v>15</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -2795,7 +2951,7 @@
         <v>16</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C34" s="16"/>
       <c r="D34" s="16"/>
@@ -2882,7 +3038,7 @@
         <v>19</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -2894,7 +3050,7 @@
         <v>6</v>
       </c>
       <c r="J37" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K37" s="18"/>
       <c r="L37" s="18"/>
@@ -2923,7 +3079,7 @@
         <v>3</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="K38" s="18"/>
       <c r="L38" s="18"/>
@@ -2940,7 +3096,7 @@
         <v>21</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C39" s="16"/>
       <c r="D39" s="16"/>
@@ -2952,7 +3108,7 @@
         <v>6</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K39" s="18"/>
       <c r="L39" s="18"/>
@@ -2981,7 +3137,7 @@
         <v>4</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K40" s="18"/>
       <c r="L40" s="18"/>
@@ -3010,7 +3166,7 @@
         <v>2</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K41" s="18"/>
       <c r="L41" s="18"/>
@@ -3039,7 +3195,7 @@
         <v>3</v>
       </c>
       <c r="J42" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K42" s="18"/>
       <c r="L42" s="18"/>
@@ -3056,7 +3212,7 @@
         <v>25</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -3068,7 +3224,7 @@
         <v>7</v>
       </c>
       <c r="J43" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K43" s="18"/>
       <c r="L43" s="18"/>
@@ -3097,7 +3253,7 @@
         <v>4</v>
       </c>
       <c r="J44" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K44" s="18"/>
       <c r="L44" s="18"/>
@@ -3126,7 +3282,7 @@
         <v>3</v>
       </c>
       <c r="J45" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K45" s="18"/>
       <c r="L45" s="18"/>
@@ -3155,7 +3311,7 @@
         <v>3</v>
       </c>
       <c r="J46" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K46" s="18"/>
       <c r="L46" s="18"/>
@@ -3184,7 +3340,7 @@
         <v>3</v>
       </c>
       <c r="J47" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K47" s="18"/>
       <c r="L47" s="18"/>
@@ -3213,7 +3369,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K48" s="18"/>
       <c r="L48" s="18"/>

</xml_diff>

<commit_message>
implemented HTTP client for downloading files
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3212BE68-5C54-44A0-B1B4-5BBDCBFB46F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4630AE-CFC6-438A-A073-793A5DF8E81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
@@ -277,26 +277,6 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* koji sadržaj preuzima aplikacija i za što je taj sadržaj potreban
-* je li prikazan tijek i postotak preuzimanja sadržaja te postoji li ograničenje brzine prijenosa podataka</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>* na se koji web servis spaja aplikacija (naziv i link), te koje njegove metode koristi</t>
     </r>
   </si>
@@ -1404,10 +1384,58 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Matija komentar:
+      <t xml:space="preserve">Matija komentar:
 Aplikacija se sapaja na freecurrencyapi, sa kojega dohvaca trenutnu vrijednost tecaja
 https://freecurrencyapi.com/
-https://github.com/everapihq/freecurrencyapi-python</t>
+https://github.com/everapihq/freecurrencyapi-python
+Sa freecurrencyapi se povlace trenutni tecajevi. Aplikacija pretvara "Sum of products price in HRK", klikom na gumb pretvara HRK u navedene valute (EUR, USD, CAD, AUD i GBP). Iako se "Sum of products price in HRK" azurira samostalno svakih 10 sec, isto nije implementirano u API call, jer postoji limit koliko se puta moze pristupiti u besplatnov inacici. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* koji sadržaj preuzima aplikacija i za što je taj sadržaj potreban
+* je li prikazan tijek i postotak preuzimanja sadržaja te postoji li ograničenje brzine prijenosa podataka
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija komentar:
+HTTP klijent implementiran kao poseban widget koji se poziva klikom na gum "Show HTTP client". Klijent je namjenjen preuzimanju slika koje se mogu dodati bazu podataka. HTTP klijent nije limitiran na skidanje slika, nego je preko njega moguce preuzeti i druge tipove podataka. Preuzeti sadrzaj se sprema u datoteku "images"
+Kada se otvori HTTP klijent korisnik unosi URL sadrzaja kojeg zeli preuzeti.
+U Speed limit edit field se moze proizvoljno unijeti brzina preuzimanja u kilobajtima. Ako se taj podatak izostavi, aplikacija preuzima sa najvecom mogucom dostupnom brzinom. Takodjer se koristniku na izbor nude 3 predefinirane brzine koje se unose pritiskom na gumb (250kbps, 500kbps, 1mbps)
+Tijek preuzimanja se prikazuje putem progress bara koji se puni prema 100%  kako se sadrzaj preuzima. Takodjer je prikazana trenutna brzina preuzimanja te koliko se datoteke preuzelo u kilobajtima (podatak se azurira kako se datoteka preuzima)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
     </r>
   </si>
 </sst>
@@ -1764,40 +1792,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1822,6 +1820,36 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2140,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:H36"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35:S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,1427 +2180,1451 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
+      <c r="A7" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
     </row>
     <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
     </row>
     <row r="18" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="20" t="s">
+      <c r="J18" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
     </row>
     <row r="19" spans="1:20" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
+      <c r="J19" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
     </row>
     <row r="20" spans="1:20" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
+      <c r="J20" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
       <c r="T20" s="12"/>
     </row>
     <row r="21" spans="1:20" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>3</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
+      <c r="J21" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
     </row>
     <row r="22" spans="1:20" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>4</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="B22" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
+      <c r="J22" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
     </row>
     <row r="23" spans="1:20" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="B23" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
+      <c r="J23" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
     </row>
     <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>6</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
+      <c r="J24" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
     </row>
     <row r="25" spans="1:20" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>7</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="24"/>
+      <c r="J25" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>8</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
+      <c r="J26" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
     </row>
     <row r="27" spans="1:20" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>9</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
+      <c r="J27" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
     </row>
     <row r="28" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>10</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+      <c r="B28" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
+      <c r="J28" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
     </row>
     <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>11</v>
       </c>
-      <c r="B29" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
+      <c r="B29" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="21"/>
-      <c r="S29" s="21"/>
+      <c r="J29" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
     </row>
     <row r="30" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>12</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
+      <c r="J30" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
     </row>
     <row r="31" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
+      <c r="B31" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="18" t="s">
+      <c r="J31" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
     </row>
     <row r="32" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>14</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="18" t="s">
+      <c r="J32" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
+      <c r="B33" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="18" t="s">
+      <c r="J33" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
+      <c r="B34" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="18" t="s">
+      <c r="J34" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
+      <c r="A35" s="10">
         <v>17</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
+      <c r="J35" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>18</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="18"/>
+      <c r="J36" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
+      <c r="B37" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
+      <c r="J37" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
     </row>
     <row r="38" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+      <c r="A38" s="10">
         <v>20</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
+      <c r="J38" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
-      <c r="B39" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
+      <c r="B39" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
+      <c r="J39" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>22</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
+      <c r="J40" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
+      <c r="J41" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
+      <c r="J42" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
+      <c r="B43" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
+      <c r="J43" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
+      <c r="J44" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
+      <c r="J45" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
+      <c r="J46" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="14"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
+      <c r="J47" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="18"/>
-      <c r="O48" s="18"/>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="18"/>
+      <c r="J48" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
-      <c r="N50" s="29"/>
-      <c r="O50" s="29"/>
-      <c r="P50" s="29"/>
-      <c r="Q50" s="29"/>
-      <c r="R50" s="29"/>
-      <c r="S50" s="29"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="30"/>
-      <c r="M51" s="30"/>
-      <c r="N51" s="30"/>
-      <c r="O51" s="30"/>
-      <c r="P51" s="30"/>
-      <c r="Q51" s="30"/>
-      <c r="R51" s="30"/>
-      <c r="S51" s="31"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="20"/>
+      <c r="O51" s="20"/>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="20"/>
+      <c r="S51" s="21"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="25"/>
-      <c r="L52" s="25"/>
-      <c r="M52" s="25"/>
-      <c r="N52" s="25"/>
-      <c r="O52" s="25"/>
-      <c r="P52" s="25"/>
-      <c r="Q52" s="25"/>
-      <c r="R52" s="25"/>
-      <c r="S52" s="26"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="15"/>
+      <c r="O52" s="15"/>
+      <c r="P52" s="15"/>
+      <c r="Q52" s="15"/>
+      <c r="R52" s="15"/>
+      <c r="S52" s="16"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
-      <c r="O53" s="25"/>
-      <c r="P53" s="25"/>
-      <c r="Q53" s="25"/>
-      <c r="R53" s="25"/>
-      <c r="S53" s="26"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="15"/>
+      <c r="S53" s="16"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
-      <c r="L54" s="25"/>
-      <c r="M54" s="25"/>
-      <c r="N54" s="25"/>
-      <c r="O54" s="25"/>
-      <c r="P54" s="25"/>
-      <c r="Q54" s="25"/>
-      <c r="R54" s="25"/>
-      <c r="S54" s="26"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+      <c r="S54" s="16"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="25"/>
-      <c r="L55" s="25"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="25"/>
-      <c r="O55" s="25"/>
-      <c r="P55" s="25"/>
-      <c r="Q55" s="25"/>
-      <c r="R55" s="25"/>
-      <c r="S55" s="26"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="15"/>
+      <c r="R55" s="15"/>
+      <c r="S55" s="16"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="27"/>
-      <c r="J56" s="27"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="27"/>
-      <c r="N56" s="27"/>
-      <c r="O56" s="27"/>
-      <c r="P56" s="27"/>
-      <c r="Q56" s="27"/>
-      <c r="R56" s="27"/>
-      <c r="S56" s="28"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="17"/>
+      <c r="R56" s="17"/>
+      <c r="S56" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B54:S54"/>
-    <mergeCell ref="B55:S55"/>
-    <mergeCell ref="B56:S56"/>
-    <mergeCell ref="J48:S48"/>
-    <mergeCell ref="A50:S50"/>
-    <mergeCell ref="B51:S51"/>
-    <mergeCell ref="B52:S52"/>
-    <mergeCell ref="B53:S53"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="J47:S47"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="J22:S22"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="J18:S18"/>
+    <mergeCell ref="J19:S19"/>
+    <mergeCell ref="J20:S20"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J24:S24"/>
+    <mergeCell ref="J25:S25"/>
+    <mergeCell ref="J26:S26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J27:S27"/>
+    <mergeCell ref="J28:S28"/>
+    <mergeCell ref="J29:S29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="J30:S30"/>
+    <mergeCell ref="J31:S31"/>
+    <mergeCell ref="J32:S32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="J34:S34"/>
+    <mergeCell ref="J35:S35"/>
     <mergeCell ref="J45:S45"/>
     <mergeCell ref="J46:S46"/>
     <mergeCell ref="B45:H45"/>
@@ -3589,48 +3641,24 @@
     <mergeCell ref="J42:S42"/>
     <mergeCell ref="J43:S43"/>
     <mergeCell ref="J44:S44"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="J34:S34"/>
-    <mergeCell ref="J35:S35"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="J30:S30"/>
-    <mergeCell ref="J31:S31"/>
-    <mergeCell ref="J32:S32"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J27:S27"/>
-    <mergeCell ref="J28:S28"/>
-    <mergeCell ref="J29:S29"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="J24:S24"/>
-    <mergeCell ref="J25:S25"/>
-    <mergeCell ref="J26:S26"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="J18:S18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="J20:S20"/>
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="A1:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B54:S54"/>
+    <mergeCell ref="B55:S55"/>
+    <mergeCell ref="B56:S56"/>
+    <mergeCell ref="J48:S48"/>
+    <mergeCell ref="A50:S50"/>
+    <mergeCell ref="B51:S51"/>
+    <mergeCell ref="B52:S52"/>
+    <mergeCell ref="B53:S53"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="J47:S47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3638,12 +3666,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7005DF65C69D244A0053930B4D80895" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfe4224a46d45a1569ee43293fdcdd48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a217f1db-afc0-486b-a03f-32483c6d35f7" xmlns:ns4="b3fc9c33-149f-45e5-9bdb-a4f7fe310215" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d8dd93a9b58d240e8e3304885c0c0fa" ns3:_="" ns4:_="">
     <xsd:import namespace="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
@@ -3860,6 +3882,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3870,23 +3898,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D0DA503-506E-48B5-9538-4DAB746C5D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3905,6 +3916,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916385B-7771-4B86-AC30-95BD0DD5FA1F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Implemented SOAP client, tested, working
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4630AE-CFC6-438A-A073-793A5DF8E81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62983829-A7EC-4DFF-9C10-E75A7BFF367D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
@@ -2168,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35:S35"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37:S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Configuration over ini files and winreq implemented
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62983829-A7EC-4DFF-9C10-E75A7BFF367D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C865A17-A55B-4DE2-B489-8920C8834B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
@@ -213,71 +213,8 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* što predstavlja procese A i B, te zašto proces A kreira (poziva) proces B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* što je povratna vrijednost procesa B</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>* koji se podaci prenose u mrežnoj komunikaciji (što šalje klijent, a što vraća poslužitelj)
 * razmjenjuju li se osim jednostavnih tipova podataka u komunikaciji i tokovi podataka (eng. streams), te što se u njima nalazi</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* na se koji web servis spaja aplikacija (naziv i link), te koje njegove metode koristi</t>
     </r>
   </si>
   <si>
@@ -733,68 +670,6 @@
 2. users.accdb
 Ova baza podataka se koristi za pohranu podataka za pristup aplikaciji (username i password). Te se sastoji od tablice 'credentials'. 
 Sve tablice podržavaju CRUD operacije (proizvodi, skladista i credentials)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Za svaki od pristupa (INI i/ili Windows registar) treba opisati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">* postavke aplikacije koji se spremaju
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Napomena: ukoliko se koriste oba pristupa (INI i Windows registar), oni moraju raditi s različitim postavkama aplikacije.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF002060"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Matija komentar:
-INI configuration file:
-Aplikacija koristi INI datoteku, te za citanje i pisanje koristi python module 'configparser'. Funkcija koja obavlja postavku se naziva 'settings' te se nalazi u python datoteci 'app.py'.
-Koristi se za tri postavke:
-1. postavke vrste fonta
-2. postavke velicine fonta
-3. postavke pozadine forme
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
     </r>
   </si>
   <si>
@@ -1373,40 +1248,6 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">* na koji se web servis spaja aplikacija (naziv i link), te koje njegove resurse koristi
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF002060"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Matija komentar:
-Aplikacija se sapaja na freecurrencyapi, sa kojega dohvaca trenutnu vrijednost tecaja
-https://freecurrencyapi.com/
-https://github.com/everapihq/freecurrencyapi-python
-Sa freecurrencyapi se povlace trenutni tecajevi. Aplikacija pretvara "Sum of products price in HRK", klikom na gumb pretvara HRK u navedene valute (EUR, USD, CAD, AUD i GBP). Iako se "Sum of products price in HRK" azurira samostalno svakih 10 sec, isto nije implementirano u API call, jer postoji limit koliko se puta moze pristupiti u besplatnov inacici. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">* koji sadržaj preuzima aplikacija i za što je taj sadržaj potreban
 * je li prikazan tijek i postotak preuzimanja sadržaja te postoji li ograničenje brzine prijenosa podataka
 </t>
@@ -1438,12 +1279,235 @@
 </t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* na koji se web servis spaja aplikacija (naziv i link), te koje njegove resurse koristi
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Matija komentar:
+Aplikacija se sapaja na freecurrencyapi, sa kojega dohvaca trenutnu vrijednost tecaja
+https://freecurrencyapi.com/
+https://github.com/everapihq/freecurrencyapi-python
+Sa freecurrencyapi se povlace trenutni tecajevi U JSON formatu. Aplikacija pretvara "Sum of products price in HRK", klikom na gumb pretvara HRK u navedene valute (EUR, USD, CAD, AUD i GBP). Iako se "Sum of products price in HRK" azurira samostalno svakih 10 sec, isto nije implementirano u API call, jer postoji limit koliko se puta moze pristupiti u besplatnov inacici. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* na se koji web servis spaja aplikacija (naziv i link), te koje njegove metode koristi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija komentar:
+SOAP komponenta aplikacije se spaja na getpostman.com bestpatan SOAP API. Koji se kosristi kako bi se dohvatila valuta ponudenih drzava prikazanih u listi 
+https://documenter.getpostman.com/view/8854915/Szf26WHn#160148f2-fbe7-4f34-bdf9-c901317171eb
+Klikom na gumb "Show SOAP client" otvara se nova forma SOAP Client. S lijeve strane se nalazi lista drzava i ISO kratica. Enter country code input field se moze unijeti ISO karatica drzave (ili klikom drzavi iz liste, pa se automatski popouni input field), klikom na gumb "Sent request" na SOAP API salje se request koji u prozoru desno ispisuje poruku sa valutom drzave te status code requesta.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* što predstavlja procese A i B, te zašto proces A kreira (poziva) proces B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* što je povratna vrijednost procesa B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Matija komentar:
+Komunikacija izmedju procesa A i B se odvija u formi "soap_client_form.py". Funkcija "send_soap_request(self)" (Process A) poziva funkciju "get_request() (process B)" koja je dio klase "SOAP_request". Proces A zapisuje podatke u widget koje mu Proces B prosljedjuje (return).
+Kada process B uspijesno zavrsi (ne rezultira greskom) vraca vrijednost "0", u suprutnome ako process B rezultira greskom (greska se hvata pomocu try and except) vraca vrijednost "1".
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Za svaki od pristupa (INI i/ili Windows registar) treba opisati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* postavke aplikacije koji se spremaju
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Napomena: ukoliko se koriste oba pristupa (INI i Windows registar), oni moraju raditi s različitim postavkama aplikacije.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Matija komentar:
+INI configuration file:
+Aplikacija koristi INI datoteku, te za citanje i pisanje koristi python module 'configparser'. Funkcija koja obavlja postavku se naziva 'settings' te se nalazi u python datoteci 'app.py'.
+Koristi se za tri postavke:
+1. postavke vrste fonta
+2. postavke velicine fonta
+3. postavke pozadine forme
+U Windows Regisry (Computer\HKEY_CURRENT_USER\Software\ntp_aplikacija)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1547,6 +1611,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1573,7 +1644,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1786,9 +1857,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1849,6 +1917,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2168,8 +2239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37:S37"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22:S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,1406 +2251,1406 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
+      <c r="A7" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="30"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="31"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="31"/>
     </row>
     <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="32"/>
-      <c r="S17" s="32"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
     </row>
     <row r="18" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="28" t="s">
+      <c r="J18" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
     </row>
     <row r="19" spans="1:20" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
+      <c r="J19" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
     </row>
     <row r="20" spans="1:20" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="12"/>
+      <c r="J20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="11"/>
     </row>
     <row r="21" spans="1:20" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="32">
         <v>3</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
+      <c r="J21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
     </row>
     <row r="22" spans="1:20" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
+      <c r="A22" s="10">
         <v>4</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="B22" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
+      <c r="J22" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
     </row>
     <row r="23" spans="1:20" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="B23" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
+      <c r="J23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
     </row>
     <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>6</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
+      <c r="J24" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
     </row>
     <row r="25" spans="1:20" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>7</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="26"/>
+      <c r="J25" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="25"/>
     </row>
     <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>8</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
+      <c r="J26" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
     </row>
     <row r="27" spans="1:20" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>9</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
+      <c r="J27" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
     </row>
     <row r="28" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>10</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="B28" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
+      <c r="J28" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
     </row>
     <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>11</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="B29" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
+      <c r="J29" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
     </row>
     <row r="30" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>12</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
+      <c r="J30" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
     </row>
     <row r="31" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="B31" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="14" t="s">
+      <c r="J31" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
     </row>
     <row r="32" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+      <c r="A32" s="10">
         <v>14</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
+      <c r="J32" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
+      <c r="B33" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
+      <c r="J33" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
+      <c r="B34" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
+      <c r="J34" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>17</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
+      <c r="J35" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13"/>
+      <c r="S35" s="13"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+      <c r="A36" s="10">
         <v>18</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="14"/>
+      <c r="J36" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
+      <c r="B37" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
-    </row>
-    <row r="38" spans="1:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="13"/>
+      <c r="S37" s="13"/>
+    </row>
+    <row r="38" spans="1:19" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>20</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
+      <c r="J38" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
-      <c r="B39" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
+      <c r="B39" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="14"/>
-      <c r="Q39" s="14"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="14"/>
+      <c r="J39" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13"/>
+      <c r="S39" s="13"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>22</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
+      <c r="J40" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="13"/>
+      <c r="S40" s="13"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="14"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="14"/>
+      <c r="J41" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
+      <c r="J42" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
+      <c r="B43" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
+      <c r="J43" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
+      <c r="J44" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="13"/>
+      <c r="P44" s="13"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="13"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="14"/>
-      <c r="P45" s="14"/>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
+      <c r="J45" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="14"/>
-      <c r="P46" s="14"/>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="14"/>
+      <c r="J46" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
-      <c r="O47" s="14"/>
-      <c r="P47" s="14"/>
-      <c r="Q47" s="14"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="14"/>
+      <c r="J47" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-      <c r="Q48" s="14"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="14"/>
+      <c r="J48" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
-      <c r="K50" s="19"/>
-      <c r="L50" s="19"/>
-      <c r="M50" s="19"/>
-      <c r="N50" s="19"/>
-      <c r="O50" s="19"/>
-      <c r="P50" s="19"/>
-      <c r="Q50" s="19"/>
-      <c r="R50" s="19"/>
-      <c r="S50" s="19"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="18"/>
+      <c r="Q50" s="18"/>
+      <c r="R50" s="18"/>
+      <c r="S50" s="18"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
-      <c r="N51" s="20"/>
-      <c r="O51" s="20"/>
-      <c r="P51" s="20"/>
-      <c r="Q51" s="20"/>
-      <c r="R51" s="20"/>
-      <c r="S51" s="21"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="19"/>
+      <c r="O51" s="19"/>
+      <c r="P51" s="19"/>
+      <c r="Q51" s="19"/>
+      <c r="R51" s="19"/>
+      <c r="S51" s="20"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-      <c r="K52" s="15"/>
-      <c r="L52" s="15"/>
-      <c r="M52" s="15"/>
-      <c r="N52" s="15"/>
-      <c r="O52" s="15"/>
-      <c r="P52" s="15"/>
-      <c r="Q52" s="15"/>
-      <c r="R52" s="15"/>
-      <c r="S52" s="16"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="14"/>
+      <c r="P52" s="14"/>
+      <c r="Q52" s="14"/>
+      <c r="R52" s="14"/>
+      <c r="S52" s="15"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
-      <c r="P53" s="15"/>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="15"/>
-      <c r="S53" s="16"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="14"/>
+      <c r="O53" s="14"/>
+      <c r="P53" s="14"/>
+      <c r="Q53" s="14"/>
+      <c r="R53" s="14"/>
+      <c r="S53" s="15"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="15"/>
-      <c r="M54" s="15"/>
-      <c r="N54" s="15"/>
-      <c r="O54" s="15"/>
-      <c r="P54" s="15"/>
-      <c r="Q54" s="15"/>
-      <c r="R54" s="15"/>
-      <c r="S54" s="16"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
+      <c r="Q54" s="14"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="15"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="15"/>
-      <c r="M55" s="15"/>
-      <c r="N55" s="15"/>
-      <c r="O55" s="15"/>
-      <c r="P55" s="15"/>
-      <c r="Q55" s="15"/>
-      <c r="R55" s="15"/>
-      <c r="S55" s="16"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="14"/>
+      <c r="P55" s="14"/>
+      <c r="Q55" s="14"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="15"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
-      <c r="J56" s="17"/>
-      <c r="K56" s="17"/>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="17"/>
-      <c r="O56" s="17"/>
-      <c r="P56" s="17"/>
-      <c r="Q56" s="17"/>
-      <c r="R56" s="17"/>
-      <c r="S56" s="18"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+      <c r="S56" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="76">

</xml_diff>

<commit_message>
Deployed REST server with HTTPS/TLS for secure sendig/recieving sensitive data. Implemented class that uses ctype and C SQLite ddl binary file. Class tested with inserting, updating and selecting data from SQLite db.
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C865A17-A55B-4DE2-B489-8920C8834B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41745F55-3E73-4438-93A0-177B7003F989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
@@ -1860,10 +1860,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1888,39 +1921,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2239,8 +2239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22:S22"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2251,1451 +2251,1427 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="30"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="29"/>
-      <c r="R15" s="29"/>
-      <c r="S15" s="29"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="31"/>
-      <c r="S16" s="31"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
     </row>
     <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="31"/>
-      <c r="R17" s="31"/>
-      <c r="S17" s="31"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
     </row>
     <row r="18" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="27" t="s">
+      <c r="J18" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="27"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
     </row>
     <row r="19" spans="1:20" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
     </row>
     <row r="20" spans="1:20" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
       <c r="T20" s="11"/>
     </row>
     <row r="21" spans="1:20" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="32">
+      <c r="A21" s="12">
         <v>3</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="J21" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
     </row>
     <row r="22" spans="1:20" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>4</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
     </row>
     <row r="23" spans="1:20" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="J23" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
     </row>
     <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>6</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
     </row>
     <row r="25" spans="1:20" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>7</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="23" t="s">
+      <c r="J25" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="25"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="24"/>
     </row>
     <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>8</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="13" t="s">
+      <c r="J26" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
     </row>
     <row r="27" spans="1:20" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>9</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="13" t="s">
+      <c r="J27" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
     </row>
     <row r="28" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>10</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="13" t="s">
+      <c r="J28" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
     </row>
     <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>11</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="13" t="s">
+      <c r="J29" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="22"/>
-      <c r="S29" s="22"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
     </row>
     <row r="30" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>12</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="13" t="s">
+      <c r="J30" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
     </row>
     <row r="31" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="13" t="s">
+      <c r="J31" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
     </row>
     <row r="32" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>14</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="13" t="s">
+      <c r="J32" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="13"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="13" t="s">
+      <c r="J33" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="13"/>
-      <c r="S33" s="13"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="13" t="s">
+      <c r="J34" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="13"/>
-      <c r="S34" s="13"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>17</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="13" t="s">
+      <c r="J35" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="13"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>18</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="13" t="s">
+      <c r="J36" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="R36" s="13"/>
-      <c r="S36" s="13"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="13" t="s">
+      <c r="J37" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
-      <c r="P37" s="13"/>
-      <c r="Q37" s="13"/>
-      <c r="R37" s="13"/>
-      <c r="S37" s="13"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
     </row>
     <row r="38" spans="1:19" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>20</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="13" t="s">
+      <c r="J38" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
-      <c r="P38" s="13"/>
-      <c r="Q38" s="13"/>
-      <c r="R38" s="13"/>
-      <c r="S38" s="13"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="18"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="13" t="s">
+      <c r="J39" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K39" s="13"/>
-      <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="13"/>
-      <c r="O39" s="13"/>
-      <c r="P39" s="13"/>
-      <c r="Q39" s="13"/>
-      <c r="R39" s="13"/>
-      <c r="S39" s="13"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>22</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="13" t="s">
+      <c r="J40" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K40" s="13"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="13"/>
-      <c r="P40" s="13"/>
-      <c r="Q40" s="13"/>
-      <c r="R40" s="13"/>
-      <c r="S40" s="13"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="13" t="s">
+      <c r="J41" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="13"/>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="13"/>
-      <c r="S41" s="13"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="13" t="s">
+      <c r="J42" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="13"/>
-      <c r="R42" s="13"/>
-      <c r="S42" s="13"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="18"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="13" t="s">
+      <c r="J43" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
-      <c r="M43" s="13"/>
-      <c r="N43" s="13"/>
-      <c r="O43" s="13"/>
-      <c r="P43" s="13"/>
-      <c r="Q43" s="13"/>
-      <c r="R43" s="13"/>
-      <c r="S43" s="13"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="13" t="s">
+      <c r="J44" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="13"/>
-      <c r="P44" s="13"/>
-      <c r="Q44" s="13"/>
-      <c r="R44" s="13"/>
-      <c r="S44" s="13"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="13" t="s">
+      <c r="J45" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="13"/>
-      <c r="O45" s="13"/>
-      <c r="P45" s="13"/>
-      <c r="Q45" s="13"/>
-      <c r="R45" s="13"/>
-      <c r="S45" s="13"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="13" t="s">
+      <c r="J46" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
-      <c r="P46" s="13"/>
-      <c r="Q46" s="13"/>
-      <c r="R46" s="13"/>
-      <c r="S46" s="13"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18"/>
+      <c r="S46" s="18"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="13" t="s">
+      <c r="J47" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="13"/>
-      <c r="O47" s="13"/>
-      <c r="P47" s="13"/>
-      <c r="Q47" s="13"/>
-      <c r="R47" s="13"/>
-      <c r="S47" s="13"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="13" t="s">
+      <c r="J48" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="K48" s="13"/>
-      <c r="L48" s="13"/>
-      <c r="M48" s="13"/>
-      <c r="N48" s="13"/>
-      <c r="O48" s="13"/>
-      <c r="P48" s="13"/>
-      <c r="Q48" s="13"/>
-      <c r="R48" s="13"/>
-      <c r="S48" s="13"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="18"/>
+      <c r="S48" s="18"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="18"/>
-      <c r="N50" s="18"/>
-      <c r="O50" s="18"/>
-      <c r="P50" s="18"/>
-      <c r="Q50" s="18"/>
-      <c r="R50" s="18"/>
-      <c r="S50" s="18"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="29"/>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="29"/>
+      <c r="Q50" s="29"/>
+      <c r="R50" s="29"/>
+      <c r="S50" s="29"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
-      <c r="J51" s="19"/>
-      <c r="K51" s="19"/>
-      <c r="L51" s="19"/>
-      <c r="M51" s="19"/>
-      <c r="N51" s="19"/>
-      <c r="O51" s="19"/>
-      <c r="P51" s="19"/>
-      <c r="Q51" s="19"/>
-      <c r="R51" s="19"/>
-      <c r="S51" s="20"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="30"/>
+      <c r="L51" s="30"/>
+      <c r="M51" s="30"/>
+      <c r="N51" s="30"/>
+      <c r="O51" s="30"/>
+      <c r="P51" s="30"/>
+      <c r="Q51" s="30"/>
+      <c r="R51" s="30"/>
+      <c r="S51" s="31"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
-      <c r="P52" s="14"/>
-      <c r="Q52" s="14"/>
-      <c r="R52" s="14"/>
-      <c r="S52" s="15"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="25"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="25"/>
+      <c r="N52" s="25"/>
+      <c r="O52" s="25"/>
+      <c r="P52" s="25"/>
+      <c r="Q52" s="25"/>
+      <c r="R52" s="25"/>
+      <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="14"/>
-      <c r="O53" s="14"/>
-      <c r="P53" s="14"/>
-      <c r="Q53" s="14"/>
-      <c r="R53" s="14"/>
-      <c r="S53" s="15"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="25"/>
+      <c r="O53" s="25"/>
+      <c r="P53" s="25"/>
+      <c r="Q53" s="25"/>
+      <c r="R53" s="25"/>
+      <c r="S53" s="26"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="14"/>
-      <c r="Q54" s="14"/>
-      <c r="R54" s="14"/>
-      <c r="S54" s="15"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="25"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="25"/>
+      <c r="N54" s="25"/>
+      <c r="O54" s="25"/>
+      <c r="P54" s="25"/>
+      <c r="Q54" s="25"/>
+      <c r="R54" s="25"/>
+      <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="14"/>
-      <c r="P55" s="14"/>
-      <c r="Q55" s="14"/>
-      <c r="R55" s="14"/>
-      <c r="S55" s="15"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="25"/>
+      <c r="K55" s="25"/>
+      <c r="L55" s="25"/>
+      <c r="M55" s="25"/>
+      <c r="N55" s="25"/>
+      <c r="O55" s="25"/>
+      <c r="P55" s="25"/>
+      <c r="Q55" s="25"/>
+      <c r="R55" s="25"/>
+      <c r="S55" s="26"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="16"/>
-      <c r="I56" s="16"/>
-      <c r="J56" s="16"/>
-      <c r="K56" s="16"/>
-      <c r="L56" s="16"/>
-      <c r="M56" s="16"/>
-      <c r="N56" s="16"/>
-      <c r="O56" s="16"/>
-      <c r="P56" s="16"/>
-      <c r="Q56" s="16"/>
-      <c r="R56" s="16"/>
-      <c r="S56" s="17"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="27"/>
+      <c r="J56" s="27"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="27"/>
+      <c r="M56" s="27"/>
+      <c r="N56" s="27"/>
+      <c r="O56" s="27"/>
+      <c r="P56" s="27"/>
+      <c r="Q56" s="27"/>
+      <c r="R56" s="27"/>
+      <c r="S56" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="A1:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A16:S17"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="J18:S18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="J20:S20"/>
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="J24:S24"/>
-    <mergeCell ref="J25:S25"/>
-    <mergeCell ref="J26:S26"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J27:S27"/>
-    <mergeCell ref="J28:S28"/>
-    <mergeCell ref="J29:S29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="J30:S30"/>
-    <mergeCell ref="J31:S31"/>
-    <mergeCell ref="J32:S32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="J34:S34"/>
-    <mergeCell ref="J35:S35"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B54:S54"/>
+    <mergeCell ref="B55:S55"/>
+    <mergeCell ref="B56:S56"/>
+    <mergeCell ref="J48:S48"/>
+    <mergeCell ref="A50:S50"/>
+    <mergeCell ref="B51:S51"/>
+    <mergeCell ref="B52:S52"/>
+    <mergeCell ref="B53:S53"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="J47:S47"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
     <mergeCell ref="J45:S45"/>
     <mergeCell ref="J46:S46"/>
     <mergeCell ref="B45:H45"/>
@@ -3712,24 +3688,48 @@
     <mergeCell ref="J42:S42"/>
     <mergeCell ref="J43:S43"/>
     <mergeCell ref="J44:S44"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B54:S54"/>
-    <mergeCell ref="B55:S55"/>
-    <mergeCell ref="B56:S56"/>
-    <mergeCell ref="J48:S48"/>
-    <mergeCell ref="A50:S50"/>
-    <mergeCell ref="B51:S51"/>
-    <mergeCell ref="B52:S52"/>
-    <mergeCell ref="B53:S53"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="J47:S47"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="J34:S34"/>
+    <mergeCell ref="J35:S35"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="J30:S30"/>
+    <mergeCell ref="J31:S31"/>
+    <mergeCell ref="J32:S32"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J27:S27"/>
+    <mergeCell ref="J28:S28"/>
+    <mergeCell ref="J29:S29"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J24:S24"/>
+    <mergeCell ref="J25:S25"/>
+    <mergeCell ref="J26:S26"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="J22:S22"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="J18:S18"/>
+    <mergeCell ref="J19:S19"/>
+    <mergeCell ref="J20:S20"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A16:S17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3737,6 +3737,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7005DF65C69D244A0053930B4D80895" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfe4224a46d45a1569ee43293fdcdd48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a217f1db-afc0-486b-a03f-32483c6d35f7" xmlns:ns4="b3fc9c33-149f-45e5-9bdb-a4f7fe310215" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d8dd93a9b58d240e8e3304885c0c0fa" ns3:_="" ns4:_="">
     <xsd:import namespace="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
@@ -3953,12 +3959,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3969,6 +3969,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D0DA503-506E-48B5-9538-4DAB746C5D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3987,23 +4004,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916385B-7771-4B86-AC30-95BD0DD5FA1F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Some minor changes to file locations. Implemented GET and POST Endpoints on the REST server. When user logs into the App, REST server sents him JWT token, that is saved to SQLite database. That token will later used for authorization of the user
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41745F55-3E73-4438-93A0-177B7003F989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761B11EF-19B7-405B-A2E4-1D39423AE28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
@@ -1863,40 +1863,10 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1921,6 +1891,36 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2240,7 +2240,7 @@
   <dimension ref="A1:T56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:H34"/>
+      <selection activeCell="J39" sqref="J39:S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2251,1427 +2251,1451 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
     </row>
     <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
     </row>
     <row r="18" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="20" t="s">
+      <c r="J18" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
     </row>
     <row r="19" spans="1:20" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="18" t="s">
+      <c r="J19" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
     </row>
     <row r="20" spans="1:20" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="J20" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
       <c r="T20" s="11"/>
     </row>
     <row r="21" spans="1:20" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>3</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="18" t="s">
+      <c r="J21" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
     </row>
     <row r="22" spans="1:20" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>4</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="18" t="s">
+      <c r="J22" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
     </row>
     <row r="23" spans="1:20" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="18" t="s">
+      <c r="J23" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
     </row>
     <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>6</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="18" t="s">
+      <c r="J24" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
     </row>
     <row r="25" spans="1:20" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>7</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="22" t="s">
+      <c r="J25" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="24"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>8</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="18" t="s">
+      <c r="J26" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
     </row>
     <row r="27" spans="1:20" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>9</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="18" t="s">
+      <c r="J27" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
     </row>
     <row r="28" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>10</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="18" t="s">
+      <c r="J28" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
     </row>
     <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>11</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="18" t="s">
+      <c r="J29" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="21"/>
-      <c r="S29" s="21"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
     </row>
     <row r="30" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>12</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="18" t="s">
+      <c r="J30" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
     </row>
     <row r="31" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="18" t="s">
+      <c r="J31" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
     </row>
     <row r="32" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>14</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="18" t="s">
+      <c r="J32" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="18" t="s">
+      <c r="J33" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="18" t="s">
+      <c r="J34" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>17</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="18" t="s">
+      <c r="J35" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>18</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="18" t="s">
+      <c r="J36" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="18"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="18" t="s">
+      <c r="J37" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
     </row>
     <row r="38" spans="1:19" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>20</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="18" t="s">
+      <c r="J38" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>21</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="18" t="s">
+      <c r="J39" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>22</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="18" t="s">
+      <c r="J40" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="18" t="s">
+      <c r="J41" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="18" t="s">
+      <c r="J42" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="18" t="s">
+      <c r="J43" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="18" t="s">
+      <c r="J44" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="18" t="s">
+      <c r="J45" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="18" t="s">
+      <c r="J46" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="14"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="18" t="s">
+      <c r="J47" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="18" t="s">
+      <c r="J48" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="18"/>
-      <c r="O48" s="18"/>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="18"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
-      <c r="N50" s="29"/>
-      <c r="O50" s="29"/>
-      <c r="P50" s="29"/>
-      <c r="Q50" s="29"/>
-      <c r="R50" s="29"/>
-      <c r="S50" s="29"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="30"/>
-      <c r="M51" s="30"/>
-      <c r="N51" s="30"/>
-      <c r="O51" s="30"/>
-      <c r="P51" s="30"/>
-      <c r="Q51" s="30"/>
-      <c r="R51" s="30"/>
-      <c r="S51" s="31"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="20"/>
+      <c r="O51" s="20"/>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="20"/>
+      <c r="S51" s="21"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="25"/>
-      <c r="L52" s="25"/>
-      <c r="M52" s="25"/>
-      <c r="N52" s="25"/>
-      <c r="O52" s="25"/>
-      <c r="P52" s="25"/>
-      <c r="Q52" s="25"/>
-      <c r="R52" s="25"/>
-      <c r="S52" s="26"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="15"/>
+      <c r="O52" s="15"/>
+      <c r="P52" s="15"/>
+      <c r="Q52" s="15"/>
+      <c r="R52" s="15"/>
+      <c r="S52" s="16"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
-      <c r="O53" s="25"/>
-      <c r="P53" s="25"/>
-      <c r="Q53" s="25"/>
-      <c r="R53" s="25"/>
-      <c r="S53" s="26"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="15"/>
+      <c r="S53" s="16"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
-      <c r="L54" s="25"/>
-      <c r="M54" s="25"/>
-      <c r="N54" s="25"/>
-      <c r="O54" s="25"/>
-      <c r="P54" s="25"/>
-      <c r="Q54" s="25"/>
-      <c r="R54" s="25"/>
-      <c r="S54" s="26"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+      <c r="S54" s="16"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="25"/>
-      <c r="L55" s="25"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="25"/>
-      <c r="O55" s="25"/>
-      <c r="P55" s="25"/>
-      <c r="Q55" s="25"/>
-      <c r="R55" s="25"/>
-      <c r="S55" s="26"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="15"/>
+      <c r="R55" s="15"/>
+      <c r="S55" s="16"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="27"/>
-      <c r="J56" s="27"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="27"/>
-      <c r="N56" s="27"/>
-      <c r="O56" s="27"/>
-      <c r="P56" s="27"/>
-      <c r="Q56" s="27"/>
-      <c r="R56" s="27"/>
-      <c r="S56" s="28"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="17"/>
+      <c r="R56" s="17"/>
+      <c r="S56" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B54:S54"/>
-    <mergeCell ref="B55:S55"/>
-    <mergeCell ref="B56:S56"/>
-    <mergeCell ref="J48:S48"/>
-    <mergeCell ref="A50:S50"/>
-    <mergeCell ref="B51:S51"/>
-    <mergeCell ref="B52:S52"/>
-    <mergeCell ref="B53:S53"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="J47:S47"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="J22:S22"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="J18:S18"/>
+    <mergeCell ref="J19:S19"/>
+    <mergeCell ref="J20:S20"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J24:S24"/>
+    <mergeCell ref="J25:S25"/>
+    <mergeCell ref="J26:S26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J27:S27"/>
+    <mergeCell ref="J28:S28"/>
+    <mergeCell ref="J29:S29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="J30:S30"/>
+    <mergeCell ref="J31:S31"/>
+    <mergeCell ref="J32:S32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="J34:S34"/>
+    <mergeCell ref="J35:S35"/>
     <mergeCell ref="J45:S45"/>
     <mergeCell ref="J46:S46"/>
     <mergeCell ref="B45:H45"/>
@@ -3688,48 +3712,24 @@
     <mergeCell ref="J42:S42"/>
     <mergeCell ref="J43:S43"/>
     <mergeCell ref="J44:S44"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="J34:S34"/>
-    <mergeCell ref="J35:S35"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="J30:S30"/>
-    <mergeCell ref="J31:S31"/>
-    <mergeCell ref="J32:S32"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J27:S27"/>
-    <mergeCell ref="J28:S28"/>
-    <mergeCell ref="J29:S29"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="J24:S24"/>
-    <mergeCell ref="J25:S25"/>
-    <mergeCell ref="J26:S26"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="J18:S18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="J20:S20"/>
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="A1:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B54:S54"/>
+    <mergeCell ref="B55:S55"/>
+    <mergeCell ref="B56:S56"/>
+    <mergeCell ref="J48:S48"/>
+    <mergeCell ref="A50:S50"/>
+    <mergeCell ref="B51:S51"/>
+    <mergeCell ref="B52:S52"/>
+    <mergeCell ref="B53:S53"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="J47:S47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3737,12 +3737,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7005DF65C69D244A0053930B4D80895" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfe4224a46d45a1569ee43293fdcdd48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a217f1db-afc0-486b-a03f-32483c6d35f7" xmlns:ns4="b3fc9c33-149f-45e5-9bdb-a4f7fe310215" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d8dd93a9b58d240e8e3304885c0c0fa" ns3:_="" ns4:_="">
     <xsd:import namespace="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
@@ -3959,6 +3953,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3969,23 +3969,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D0DA503-506E-48B5-9538-4DAB746C5D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4004,6 +3987,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916385B-7771-4B86-AC30-95BD0DD5FA1F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Implemented REST server fully, it is hosted online
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761B11EF-19B7-405B-A2E4-1D39423AE28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF499C83-2815-44B5-B13C-62EC4342F456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
@@ -311,7 +311,8 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* na koji se način provodi autentifikacija i autorizacija, te koje ovlasti ima svaki od korisnika</t>
+      <t>* koje se funkcije/klase/metode nalaze u statičkoj biblioteci
+* u koju se svrhu koriste navedene funkcije/klase/metode</t>
     </r>
   </si>
   <si>
@@ -330,8 +331,8 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* koje se funkcije/klase/metode nalaze u statičkoj biblioteci
-* u koju se svrhu koriste navedene funkcije/klase/metode</t>
+      <t>* u koju se svrhu koristi web servis te koje su njegove metode
+* je li web servis smješten na web poslužitelju (IIS, Apache ili sl.) ili u zasebnoj (desktop) aplikaciji</t>
     </r>
   </si>
   <si>
@@ -350,13 +351,18 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* u koju se svrhu koristi web servis te koje su njegove metode
-* je li web servis smješten na web poslužitelju (IIS, Apache ili sl.) ili u zasebnoj (desktop) aplikaciji</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
+      <t>* koji su sve jezici podržani</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -370,18 +376,12 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* koji su sve jezici podržani</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+      <t>* koliko dijaloga je prevedeno</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
 </t>
     </r>
     <r>
@@ -395,25 +395,6 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* koliko dijaloga je prevedeno</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">* koji se podaci šifriraju i dešifriraju u aplikaciji
 </t>
     </r>
@@ -427,27 +408,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Napomena: lozinke se ne šifriraju!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* u koju se svrhu koristi web servis
-* koje resurse te koje metode nudi nad svakim od resursa (GET, PUT, …)
-* je li web servis smješten na web poslužitelju (IIS, Apache ili sl.) ili u zasebnoj (desktop) aplikaciji</t>
     </r>
   </si>
   <si>
@@ -1502,12 +1462,127 @@
 </t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* u koju se svrhu koristi web servis
+* koje resurse te koje metode nudi nad svakim od resursa (GET, PUT, …)
+* je li web servis smješten na web poslužitelju (IIS, Apache ili sl.) ili u zasebnoj (desktop) aplikaciji
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Matija komentar:
+Rest server je hostan na https://www.pythonanywhere.com/, REST server URL https://nitroblaze.pythonanywhere.com/, kada se otvori ovaj link, javlja gresku "Not Found", to je zato sto nije definiran index.html za pocetnu stranicu, api callovi rade npr. https://nitroblaze.pythonanywhere.com/api/protected vraca json {"message":"Token missing"}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rest server: 
+@app.route('/api/get_token', methods=['GET']) - useru se pri login-u u aplikaciju dodijeli JWT token za autorizaciju
+@app.route('/api/protected', methods=['GET'])- vraca listu korisne informacije za admin usera, kao sto su informacije vezane za API 
+@app.route('/api/logistic_partners', methods=['GET']) - vraca listu logistickih partnera
+@app.route('/api/logistic_partners', methods=['POST']) - postavlja novi parametar u listu logistickih partnera</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* na koji se način provodi autentifikacija i autorizacija, te koje ovlasti ima svaki od korisnika</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija komentar:
+Korisik kod logina dovije JWT token, koji se spremi u SQLite bazu. Korisnik kada na REST server formi klikne na Admin, aplikacija salje korisnikov JWT token REST serveru  na autorizaciju. REST server po JWT tokenu zna o kojem se useru radi, te ovisno o useru vrati JSON. Ako je admin dobije resurs, ako je bilo koji drugi user dobije poruku unauthorized.
+JWT token se kod generacije kriptira, te takav salje useru, kada se vrati REST serveru, server ga desifira i iz njega procita o kojem se useru radi. Rest server koristi HS256 simetricni alogiram.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1616,6 +1691,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1863,10 +1953,40 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1891,36 +2011,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2239,8 +2329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39:S39"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="T40" sqref="T40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2251,1451 +2341,1427 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
+      <c r="A7" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="31"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
     </row>
     <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="32"/>
-      <c r="S17" s="32"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
     </row>
     <row r="18" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="28" t="s">
+      <c r="J18" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
     </row>
     <row r="19" spans="1:20" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>1</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
+      <c r="J19" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
     </row>
     <row r="20" spans="1:20" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
+      <c r="J20" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
       <c r="T20" s="11"/>
     </row>
     <row r="21" spans="1:20" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>3</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
+      <c r="J21" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
     </row>
     <row r="22" spans="1:20" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>4</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="B22" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
+      <c r="J22" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
     </row>
     <row r="23" spans="1:20" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="B23" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
+      <c r="J23" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
     </row>
     <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>6</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
+      <c r="J24" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
     </row>
     <row r="25" spans="1:20" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>7</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="26"/>
+      <c r="J25" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="24"/>
     </row>
     <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>8</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
+      <c r="J26" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
     </row>
     <row r="27" spans="1:20" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>9</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
+      <c r="J27" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
     </row>
     <row r="28" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>10</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="B28" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
+      <c r="J28" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
     </row>
     <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>11</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="B29" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
+      <c r="J29" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
     </row>
     <row r="30" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>12</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
+      <c r="J30" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
     </row>
     <row r="31" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="B31" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="14" t="s">
+      <c r="J31" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
     </row>
     <row r="32" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>14</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
+      <c r="J32" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
+      <c r="B33" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="J33" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
+      <c r="B34" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="14" t="s">
+      <c r="J34" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>17</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
+      <c r="J35" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>18</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="14"/>
+      <c r="J36" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
+      <c r="B37" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
+      <c r="J37" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
     </row>
     <row r="38" spans="1:19" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>20</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
+      <c r="J38" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="18"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
+      <c r="A39" s="10">
         <v>21</v>
       </c>
-      <c r="B39" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
+      <c r="B39" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="14"/>
-      <c r="Q39" s="14"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="14"/>
+      <c r="J39" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
+      <c r="A40" s="10">
         <v>22</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
+      <c r="J40" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="14"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="14"/>
+      <c r="J41" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
+      <c r="J42" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="18"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
+      <c r="B43" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
+      <c r="J43" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="14" t="s">
+      <c r="J44" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="14"/>
-      <c r="P45" s="14"/>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
+      <c r="J45" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
     </row>
     <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="14" t="s">
+      <c r="J46" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="14"/>
-      <c r="P46" s="14"/>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="14"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18"/>
+      <c r="S46" s="18"/>
     </row>
     <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="14" t="s">
+      <c r="J47" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
-      <c r="O47" s="14"/>
-      <c r="P47" s="14"/>
-      <c r="Q47" s="14"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="14"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
     </row>
     <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>30</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="14" t="s">
+      <c r="J48" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-      <c r="Q48" s="14"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="14"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="18"/>
+      <c r="S48" s="18"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
-      <c r="K50" s="19"/>
-      <c r="L50" s="19"/>
-      <c r="M50" s="19"/>
-      <c r="N50" s="19"/>
-      <c r="O50" s="19"/>
-      <c r="P50" s="19"/>
-      <c r="Q50" s="19"/>
-      <c r="R50" s="19"/>
-      <c r="S50" s="19"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="29"/>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="29"/>
+      <c r="Q50" s="29"/>
+      <c r="R50" s="29"/>
+      <c r="S50" s="29"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
-      <c r="N51" s="20"/>
-      <c r="O51" s="20"/>
-      <c r="P51" s="20"/>
-      <c r="Q51" s="20"/>
-      <c r="R51" s="20"/>
-      <c r="S51" s="21"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="30"/>
+      <c r="L51" s="30"/>
+      <c r="M51" s="30"/>
+      <c r="N51" s="30"/>
+      <c r="O51" s="30"/>
+      <c r="P51" s="30"/>
+      <c r="Q51" s="30"/>
+      <c r="R51" s="30"/>
+      <c r="S51" s="31"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-      <c r="K52" s="15"/>
-      <c r="L52" s="15"/>
-      <c r="M52" s="15"/>
-      <c r="N52" s="15"/>
-      <c r="O52" s="15"/>
-      <c r="P52" s="15"/>
-      <c r="Q52" s="15"/>
-      <c r="R52" s="15"/>
-      <c r="S52" s="16"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="25"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="25"/>
+      <c r="N52" s="25"/>
+      <c r="O52" s="25"/>
+      <c r="P52" s="25"/>
+      <c r="Q52" s="25"/>
+      <c r="R52" s="25"/>
+      <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
-      <c r="P53" s="15"/>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="15"/>
-      <c r="S53" s="16"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="25"/>
+      <c r="O53" s="25"/>
+      <c r="P53" s="25"/>
+      <c r="Q53" s="25"/>
+      <c r="R53" s="25"/>
+      <c r="S53" s="26"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="15"/>
-      <c r="M54" s="15"/>
-      <c r="N54" s="15"/>
-      <c r="O54" s="15"/>
-      <c r="P54" s="15"/>
-      <c r="Q54" s="15"/>
-      <c r="R54" s="15"/>
-      <c r="S54" s="16"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="25"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="25"/>
+      <c r="N54" s="25"/>
+      <c r="O54" s="25"/>
+      <c r="P54" s="25"/>
+      <c r="Q54" s="25"/>
+      <c r="R54" s="25"/>
+      <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="15"/>
-      <c r="M55" s="15"/>
-      <c r="N55" s="15"/>
-      <c r="O55" s="15"/>
-      <c r="P55" s="15"/>
-      <c r="Q55" s="15"/>
-      <c r="R55" s="15"/>
-      <c r="S55" s="16"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="25"/>
+      <c r="K55" s="25"/>
+      <c r="L55" s="25"/>
+      <c r="M55" s="25"/>
+      <c r="N55" s="25"/>
+      <c r="O55" s="25"/>
+      <c r="P55" s="25"/>
+      <c r="Q55" s="25"/>
+      <c r="R55" s="25"/>
+      <c r="S55" s="26"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
-      <c r="J56" s="17"/>
-      <c r="K56" s="17"/>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="17"/>
-      <c r="O56" s="17"/>
-      <c r="P56" s="17"/>
-      <c r="Q56" s="17"/>
-      <c r="R56" s="17"/>
-      <c r="S56" s="18"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="27"/>
+      <c r="J56" s="27"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="27"/>
+      <c r="M56" s="27"/>
+      <c r="N56" s="27"/>
+      <c r="O56" s="27"/>
+      <c r="P56" s="27"/>
+      <c r="Q56" s="27"/>
+      <c r="R56" s="27"/>
+      <c r="S56" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="A1:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A16:S17"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="J18:S18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="J20:S20"/>
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="J24:S24"/>
-    <mergeCell ref="J25:S25"/>
-    <mergeCell ref="J26:S26"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J27:S27"/>
-    <mergeCell ref="J28:S28"/>
-    <mergeCell ref="J29:S29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="J30:S30"/>
-    <mergeCell ref="J31:S31"/>
-    <mergeCell ref="J32:S32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="J34:S34"/>
-    <mergeCell ref="J35:S35"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B54:S54"/>
+    <mergeCell ref="B55:S55"/>
+    <mergeCell ref="B56:S56"/>
+    <mergeCell ref="J48:S48"/>
+    <mergeCell ref="A50:S50"/>
+    <mergeCell ref="B51:S51"/>
+    <mergeCell ref="B52:S52"/>
+    <mergeCell ref="B53:S53"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="J47:S47"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
     <mergeCell ref="J45:S45"/>
     <mergeCell ref="J46:S46"/>
     <mergeCell ref="B45:H45"/>
@@ -3712,24 +3778,48 @@
     <mergeCell ref="J42:S42"/>
     <mergeCell ref="J43:S43"/>
     <mergeCell ref="J44:S44"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B54:S54"/>
-    <mergeCell ref="B55:S55"/>
-    <mergeCell ref="B56:S56"/>
-    <mergeCell ref="J48:S48"/>
-    <mergeCell ref="A50:S50"/>
-    <mergeCell ref="B51:S51"/>
-    <mergeCell ref="B52:S52"/>
-    <mergeCell ref="B53:S53"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="J47:S47"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="J34:S34"/>
+    <mergeCell ref="J35:S35"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="J30:S30"/>
+    <mergeCell ref="J31:S31"/>
+    <mergeCell ref="J32:S32"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J27:S27"/>
+    <mergeCell ref="J28:S28"/>
+    <mergeCell ref="J29:S29"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J24:S24"/>
+    <mergeCell ref="J25:S25"/>
+    <mergeCell ref="J26:S26"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="J22:S22"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="J18:S18"/>
+    <mergeCell ref="J19:S19"/>
+    <mergeCell ref="J20:S20"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A16:S17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3737,6 +3827,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7005DF65C69D244A0053930B4D80895" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfe4224a46d45a1569ee43293fdcdd48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a217f1db-afc0-486b-a03f-32483c6d35f7" xmlns:ns4="b3fc9c33-149f-45e5-9bdb-a4f7fe310215" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d8dd93a9b58d240e8e3304885c0c0fa" ns3:_="" ns4:_="">
     <xsd:import namespace="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
@@ -3953,12 +4049,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3969,6 +4059,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D0DA503-506E-48B5-9538-4DAB746C5D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3987,23 +4094,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916385B-7771-4B86-AC30-95BD0DD5FA1F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Implemented PasswordHashing on passwords that are saved in database so they do not show as PlainText. Added translation for five languages: Croatian, English, German, Spanish and French.
</commit_message>
<xml_diff>
--- a/matija_stanic_prijavnica.xlsx
+++ b/matija_stanic_prijavnica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matija\Desktop\NTP - project\pain-and-suffering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF499C83-2815-44B5-B13C-62EC4342F456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF66F62D-4362-4E81-8F32-512793370498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E3D7DB7-27B3-4496-A59A-1903852127ED}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -253,130 +253,8 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* koje se funkcije/klase/metode nalaze u dinamičkoj biblioteci
-* u koju se svrhu koriste navedene funkcije/klase/metode</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* koji se dijalozi nalaze u dinamičkoj biblioteci, te u koju svrhu se koriste</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* koji se resursi nalaze u dinamičkoj biblioteci, te u koju svrhu se koriste</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* koje se funkcije/klase/metode nalaze u statičkoj biblioteci
-* u koju se svrhu koriste navedene funkcije/klase/metode</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>* u koju se svrhu koristi web servis te koje su njegove metode
 * je li web servis smješten na web poslužitelju (IIS, Apache ili sl.) ili u zasebnoj (desktop) aplikaciji</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* koji su sve jezici podržani</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* koliko dijaloga je prevedeno</t>
     </r>
   </si>
   <si>
@@ -504,52 +382,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Važno! Prijavnica se nastavniku šalje na pregled i odobrenje samo ukoliko suma bodova po odabranim funkcionalnostima iznosi minimalno 51 bod!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* što se sažima
-* koristi li se "sol", te je li fiksna ili promjenjiva
-* ako je "sol" promjenjiva, na koji način (po kojem pravilu) se generira</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* da li se koristi "papar" i na koji način se vrši njegova provjera</t>
     </r>
   </si>
   <si>
@@ -853,51 +685,6 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">* nazive klasa, atributa i metoda (ukoliko projekt sadrži mnogo klasa/atributa/metoda dovoljno je navesti samo 3 klase s po minimalno 2 atributa i metode)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Napomena: priznaju se samo klase koje je student napisao (ne priznaju se automatski generirane klase od strane razvojnog okruženja/programskog jezika).
-Matija</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Opis treba sadržavati:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>* koje se operacije izvršavaju paralelno, tj. korištenjem više dretvi</t>
     </r>
     <r>
@@ -1574,6 +1361,370 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* koji se dijalozi nalaze u dinamičkoj biblioteci, te u koju svrhu se koriste
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija komentar:
+Aplikacija koristi SQL lite dijallog (sqlite3.dll), on se koristi kako bi aplikacija mogla komunicirati sa sqlite bazompodataka u koju se spremaju JWT tokeni za autorizaciju usera sa REST serverom</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* koji se resursi nalaze u dinamičkoj biblioteci, te u koju svrhu se koriste
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Matija komentar:
+Neki od resursa koji se koriste su funckije sqlite3_open_v2 koja otvara konekciju sa bazom podataka I sqlite3_exec koja izvrsi upit nad bazom podataka, sqlite3_close funkcija koja zatvara konekciju sa bazom, ... 
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* što se sažima
+* koristi li se "sol", te je li fiksna ili promjenjiva
+* ako je "sol" promjenjiva, na koji način (po kojem pravilu) se generira</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* da li se koristi "papar" i na koji način se vrši njegova provjera</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija komentar:
+Što se sažima:
+Lozinka se sažima korištenjem algoritma SHA-256, što rezultira jedinstvenim dugim nizom znakova (hash vrijednost).
+Koristi li se "sol", te je li fiksna ili promjenjiva, te gdje se sprema:
+Da, koristi se sol. Sol je promjenjiva i generira se pomoću funkcije generate_salt(). Svaki put kad se kreira hash lozinke, generira se nova sol. Sol se sprema zajedno s hashiranim lozinkom u formatu: salt$hashed_password.
+Ako je "sol" promjenjiva, na koji način (po kojem pravilu) se generira:
+Sol se generira pomoću funkcije generate_salt(), koja koristi token_urlsafe(20) za generiranje slučajnog niza od 20 znakova. Ovo osigurava da je svaka sol jedinstvena i slučajna.
+Da li se koristi "papar" i na koji način se vrši njegova provjera:
+Da, koristi se "papar". Papar se čita iz JSON datoteke pepper.json pomoću funkcije generate_pepper(). Funkcija odabire jedan slučajni papar iz popisa papara u JSON datoteci. Zatim se papar koristi zajedno s soli i unesenom lozinkom za stvaranje hash vrijednosti lozinke.
+Prilikom provjere lozinke u funkciji verify_password(), za svaki papar iz popisa papara pokušava se stvoriti hash lozinke s unesenom lozinkom, solju i tim paprom. Zatim se ta hash vrijednost uspoređuje s hash vrijednošću koja je spremljena u bazi podataka. Ako se podudaraju, lozinka je ispravna; inače je lozinka netočna.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* koji su sve jezici podržani</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* koliko dijaloga je prevedeno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija komentar:
+Aplikacija podrzava Hrvatski, Engleski, Njemacki, Spanjolski I Francuski jezik. Svi dijalozi osim popup messega kao sto su Error Message, Info Message, ...</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* nazive klasa, atributa i metoda (ukoliko projekt sadrži mnogo klasa/atributa/metoda dovoljno je navesti samo 3 klase s po minimalno 2 atributa i metode)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Napomena: priznaju se samo klase koje je student napisao (ne priznaju se automatski generirane klase od strane razvojnog okruženja/programskog jezika).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija komentar:
+Aplikacija sadrzi vise klasa, atributa i metoda:
+Nalazi se u main_form.py:
+class Report_Generator() - generiranje reporta - 
+def get_product_data() - prikazuje ili generira report ovisno o klicku na app GUI
+def get_master_detail_data() - prikazuje ili generira report ovisno o klicku na app GUI
+self.product_data - za spremanje podataka iz baze
+self.master_detail_data - za spremanje podataka iz baze
+class ParallelTaskExecutor() - multithreading sa bazenom dretvi  za generiranje reporta
+def run_tasks() - pokrece taskove
+def shutdown() - gasi procese
+self.max_workers - koliko se koristi dretvi
+self.executor
+class getAPIRequest()
+self.api_key - API key za online SOAP posluzitelj
+self.api_result - sluzi za spremanje rezultata 
+def get_api_resultdef() - dohvaca rezultate sa servera
+def return_api_result() - sluzi za zapisivanje rezultata</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* koje se funkcije/klase/metode nalaze u dinamičkoj biblioteci
+* u koju se svrhu koriste navedene funkcije/klase/metode
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Matija Komentar:
+Aplikaciju i dinamicku biblijoteku sqlite3.dll povezuje modul "ctypes". DLL se koristi kako bi se u SQLite databazu zapisivao JWT token koji sluzi za authorizaciju usera na REST serveru.
+Clijeli programski kod oko sqlite3.dll  je implementiran kao klasa class JwtDatabaseManager() koja sadrzi funkcije:
+def update_or_insert_jwt() - azurira token u databazi ako postoji, ako ne onda zapise vrijednost
+def select_all_from_table()  - ispisuje sve vrijendnosti iz tablice
+def get_jwt_for_username() - ispisuje JWT token iz tablice ovisno o usernameu
+Iz DLL datoteke se uz moju klasku koriste i built-in funkcije:
+funkcije: sqlite3_open_v2, sqlite3_exec, sqlite3_close</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opis treba sadržavati:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* koje se funkcije/klase/metode nalaze u statičkoj biblioteci
+* u koju se svrhu koriste navedene funkcije/klase/metode
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Matija komentar:
+U pythonu ne postoje staticne biblioteke kao u CPP, to bi u Pythonu bili moduli koje sam ja napravio.
+Moja aplikacija se temelji na custom modulima koji obavljaju razlicite svrhe
+1. access_connector.py - koristi se za povezivanje aplikacije sa bazom podataka MS Access
+def user_database() - ispisuje sve username iz tablice credentials
+def delete_product_by_id() - brise proizvod po ID proizvoda
+def delete_warehouse_by_id() - brise skladiste ovisno o ID skladista
+def delete_user_from_database() - brise korisnika iz tablice credentials
+2. winreg_utils.py - povezivanje WinRegistry i aplikacije za spremanje postavka aplikacije
+def win_reg_app_data() - dohvaca sve vrijednosti iz Registry patha Computer\HKEY_CURRENT_USER\Software\ntp_aplikacija 
+3. sqlite3dll_handler_class.py - povezivanje SQLite baze i aplikacije
+class JwtDatabaseManager()
+def update_or_insert_jwt()
+select_all_from_table()
+get_jwt_for_username()
+4
 </t>
     </r>
   </si>
@@ -1709,7 +1860,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1729,12 +1880,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1950,43 +2095,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2011,6 +2123,39 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2329,8 +2474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6689B64-C06F-4EF3-9A6F-7B6BB9FDA467}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="T40" sqref="T40"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32:S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2341,1427 +2486,1451 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
+      <c r="A7" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="30"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
     </row>
     <row r="13" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="31"/>
     </row>
     <row r="17" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
     </row>
     <row r="18" spans="1:20" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
       <c r="I18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="20" t="s">
+      <c r="J18" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
     </row>
     <row r="19" spans="1:20" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="10">
         <v>1</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
       <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
+      <c r="J19" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
     </row>
     <row r="20" spans="1:20" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
       <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
+      <c r="J20" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
       <c r="T20" s="11"/>
     </row>
     <row r="21" spans="1:20" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
+      <c r="A21" s="32">
         <v>3</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
       <c r="I21" s="4">
         <v>4</v>
       </c>
-      <c r="J21" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
+      <c r="J21" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
     </row>
     <row r="22" spans="1:20" ht="82.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>4</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="B22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
       <c r="I22" s="4">
         <v>4</v>
       </c>
-      <c r="J22" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
+      <c r="J22" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
     </row>
     <row r="23" spans="1:20" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="B23" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
       <c r="I23" s="4">
         <v>6</v>
       </c>
-      <c r="J23" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
+      <c r="J23" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
     </row>
     <row r="24" spans="1:20" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>6</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
       <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
+      <c r="J24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
     </row>
     <row r="25" spans="1:20" ht="372.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>7</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
       <c r="I25" s="4">
         <v>5</v>
       </c>
-      <c r="J25" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="24"/>
+      <c r="J25" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="25"/>
     </row>
     <row r="26" spans="1:20" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>8</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
       <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
+      <c r="J26" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
     </row>
     <row r="27" spans="1:20" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>9</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
       <c r="I27" s="4">
         <v>3</v>
       </c>
-      <c r="J27" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
+      <c r="J27" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
     </row>
     <row r="28" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>10</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+      <c r="B28" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
       <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
+      <c r="J28" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
     </row>
     <row r="29" spans="1:20" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>11</v>
       </c>
-      <c r="B29" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
+      <c r="B29" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
       <c r="I29" s="4">
         <v>5</v>
       </c>
-      <c r="J29" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="21"/>
-      <c r="S29" s="21"/>
+      <c r="J29" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
     </row>
     <row r="30" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>12</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
       <c r="I30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
+      <c r="J30" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
     </row>
     <row r="31" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>13</v>
       </c>
-      <c r="B31" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
+      <c r="B31" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
       <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="18" t="s">
+      <c r="J31" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
     </row>
     <row r="32" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>14</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
       <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J32" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
+      <c r="J32" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
     </row>
     <row r="33" spans="1:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>15</v>
       </c>
-      <c r="B33" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
+      <c r="B33" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
       <c r="I33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="18" t="s">
+      <c r="J33" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
     </row>
     <row r="34" spans="1:19" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>16</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
+      <c r="B34" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
       <c r="I34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="18" t="s">
+      <c r="J34" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
     </row>
     <row r="35" spans="1:19" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>17</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
       <c r="I35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
+      <c r="J35" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13"/>
+      <c r="S35" s="13"/>
     </row>
     <row r="36" spans="1:19" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>18</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
       <c r="I36" s="4">
         <v>3</v>
       </c>
-      <c r="J36" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="18"/>
+      <c r="J36" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
     </row>
     <row r="37" spans="1:19" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>19</v>
       </c>
-      <c r="B37" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
+      <c r="B37" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
       <c r="I37" s="4">
         <v>6</v>
       </c>
-      <c r="J37" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
+      <c r="J37" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="13"/>
+      <c r="S37" s="13"/>
     </row>
     <row r="38" spans="1:19" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>20</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
       <c r="I38" s="4">
         <v>3</v>
       </c>
-      <c r="J38" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
+      <c r="J38" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
     </row>
     <row r="39" spans="1:19" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>21</v>
       </c>
-      <c r="B39" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
+      <c r="B39" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
       <c r="I39" s="4">
         <v>6</v>
       </c>
-      <c r="J39" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
+      <c r="J39" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13"/>
+      <c r="S39" s="13"/>
     </row>
     <row r="40" spans="1:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>22</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
       <c r="I40" s="4">
         <v>4</v>
       </c>
-      <c r="J40" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
+      <c r="J40" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="13"/>
+      <c r="S40" s="13"/>
     </row>
     <row r="41" spans="1:19" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>23</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
       <c r="I41" s="3">
         <v>2</v>
       </c>
-      <c r="J41" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
+      <c r="J41" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
     </row>
     <row r="42" spans="1:19" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>24</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
       <c r="I42" s="3">
         <v>3</v>
       </c>
-      <c r="J42" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
+      <c r="J42" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
     </row>
     <row r="43" spans="1:19" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
+      <c r="A43" s="10">
         <v>25</v>
       </c>
-      <c r="B43" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
+      <c r="B43" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
       <c r="I43" s="3">
         <v>7</v>
       </c>
-      <c r="J43" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
+      <c r="J43" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
     </row>
     <row r="44" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>26</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
       <c r="I44" s="3">
         <v>4</v>
       </c>
-      <c r="J44" s="18" t="s">
+      <c r="J44" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="13"/>
+      <c r="P44" s="13"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="13"/>
     </row>
     <row r="45" spans="1:19" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
+      <c r="A45" s="10">
         <v>27</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
       <c r="I45" s="3">
         <v>3</v>
       </c>
-      <c r="J45" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
-    </row>
-    <row r="46" spans="1:19" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
+      <c r="J45" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
+    </row>
+    <row r="46" spans="1:19" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
         <v>28</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
       <c r="I46" s="3">
         <v>3</v>
       </c>
-      <c r="J46" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
-    </row>
-    <row r="47" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
+      <c r="J46" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
+    </row>
+    <row r="47" spans="1:19" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="10">
         <v>29</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
       <c r="I47" s="3">
         <v>3</v>
       </c>
-      <c r="J47" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
-    </row>
-    <row r="48" spans="1:19" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
+      <c r="J47" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13"/>
+    </row>
+    <row r="48" spans="1:19" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
         <v>30</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
       <c r="I48" s="3">
         <v>2</v>
       </c>
-      <c r="J48" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="18"/>
-      <c r="O48" s="18"/>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="18"/>
+      <c r="J48" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
-      <c r="N50" s="29"/>
-      <c r="O50" s="29"/>
-      <c r="P50" s="29"/>
-      <c r="Q50" s="29"/>
-      <c r="R50" s="29"/>
-      <c r="S50" s="29"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="18"/>
+      <c r="Q50" s="18"/>
+      <c r="R50" s="18"/>
+      <c r="S50" s="18"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>31</v>
       </c>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="30"/>
-      <c r="M51" s="30"/>
-      <c r="N51" s="30"/>
-      <c r="O51" s="30"/>
-      <c r="P51" s="30"/>
-      <c r="Q51" s="30"/>
-      <c r="R51" s="30"/>
-      <c r="S51" s="31"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="19"/>
+      <c r="O51" s="19"/>
+      <c r="P51" s="19"/>
+      <c r="Q51" s="19"/>
+      <c r="R51" s="19"/>
+      <c r="S51" s="20"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>32</v>
       </c>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="25"/>
-      <c r="L52" s="25"/>
-      <c r="M52" s="25"/>
-      <c r="N52" s="25"/>
-      <c r="O52" s="25"/>
-      <c r="P52" s="25"/>
-      <c r="Q52" s="25"/>
-      <c r="R52" s="25"/>
-      <c r="S52" s="26"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="14"/>
+      <c r="P52" s="14"/>
+      <c r="Q52" s="14"/>
+      <c r="R52" s="14"/>
+      <c r="S52" s="15"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>33</v>
       </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
-      <c r="O53" s="25"/>
-      <c r="P53" s="25"/>
-      <c r="Q53" s="25"/>
-      <c r="R53" s="25"/>
-      <c r="S53" s="26"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="14"/>
+      <c r="O53" s="14"/>
+      <c r="P53" s="14"/>
+      <c r="Q53" s="14"/>
+      <c r="R53" s="14"/>
+      <c r="S53" s="15"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>34</v>
       </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
-      <c r="L54" s="25"/>
-      <c r="M54" s="25"/>
-      <c r="N54" s="25"/>
-      <c r="O54" s="25"/>
-      <c r="P54" s="25"/>
-      <c r="Q54" s="25"/>
-      <c r="R54" s="25"/>
-      <c r="S54" s="26"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
+      <c r="Q54" s="14"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="15"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>35</v>
       </c>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="25"/>
-      <c r="L55" s="25"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="25"/>
-      <c r="O55" s="25"/>
-      <c r="P55" s="25"/>
-      <c r="Q55" s="25"/>
-      <c r="R55" s="25"/>
-      <c r="S55" s="26"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="14"/>
+      <c r="P55" s="14"/>
+      <c r="Q55" s="14"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="15"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="27"/>
-      <c r="J56" s="27"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="27"/>
-      <c r="N56" s="27"/>
-      <c r="O56" s="27"/>
-      <c r="P56" s="27"/>
-      <c r="Q56" s="27"/>
-      <c r="R56" s="27"/>
-      <c r="S56" s="28"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+      <c r="S56" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B54:S54"/>
-    <mergeCell ref="B55:S55"/>
-    <mergeCell ref="B56:S56"/>
-    <mergeCell ref="J48:S48"/>
-    <mergeCell ref="A50:S50"/>
-    <mergeCell ref="B51:S51"/>
-    <mergeCell ref="B52:S52"/>
-    <mergeCell ref="B53:S53"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="J47:S47"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="A1:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A6:S6"/>
+    <mergeCell ref="A7:S13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A15:S15"/>
+    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="J22:S22"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="J18:S18"/>
+    <mergeCell ref="J19:S19"/>
+    <mergeCell ref="J20:S20"/>
+    <mergeCell ref="J21:S21"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J24:S24"/>
+    <mergeCell ref="J25:S25"/>
+    <mergeCell ref="J26:S26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J27:S27"/>
+    <mergeCell ref="J28:S28"/>
+    <mergeCell ref="J29:S29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="J30:S30"/>
+    <mergeCell ref="J31:S31"/>
+    <mergeCell ref="J32:S32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="J34:S34"/>
+    <mergeCell ref="J35:S35"/>
     <mergeCell ref="J45:S45"/>
     <mergeCell ref="J46:S46"/>
     <mergeCell ref="B45:H45"/>
@@ -3778,48 +3947,24 @@
     <mergeCell ref="J42:S42"/>
     <mergeCell ref="J43:S43"/>
     <mergeCell ref="J44:S44"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="J34:S34"/>
-    <mergeCell ref="J35:S35"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="J30:S30"/>
-    <mergeCell ref="J31:S31"/>
-    <mergeCell ref="J32:S32"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J27:S27"/>
-    <mergeCell ref="J28:S28"/>
-    <mergeCell ref="J29:S29"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="J24:S24"/>
-    <mergeCell ref="J25:S25"/>
-    <mergeCell ref="J26:S26"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="J18:S18"/>
-    <mergeCell ref="J19:S19"/>
-    <mergeCell ref="J20:S20"/>
-    <mergeCell ref="J21:S21"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="A1:S3"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A6:S6"/>
-    <mergeCell ref="A7:S13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="A15:S15"/>
-    <mergeCell ref="A16:S17"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B54:S54"/>
+    <mergeCell ref="B55:S55"/>
+    <mergeCell ref="B56:S56"/>
+    <mergeCell ref="J48:S48"/>
+    <mergeCell ref="A50:S50"/>
+    <mergeCell ref="B51:S51"/>
+    <mergeCell ref="B52:S52"/>
+    <mergeCell ref="B53:S53"/>
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="J47:S47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3827,12 +3972,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7005DF65C69D244A0053930B4D80895" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfe4224a46d45a1569ee43293fdcdd48">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a217f1db-afc0-486b-a03f-32483c6d35f7" xmlns:ns4="b3fc9c33-149f-45e5-9bdb-a4f7fe310215" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d8dd93a9b58d240e8e3304885c0c0fa" ns3:_="" ns4:_="">
     <xsd:import namespace="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
@@ -4049,6 +4188,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4059,23 +4204,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D0DA503-506E-48B5-9538-4DAB746C5D15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4094,6 +4222,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B824CF8-C886-4B4F-A487-88AF19B36662}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b3fc9c33-149f-45e5-9bdb-a4f7fe310215"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a217f1db-afc0-486b-a03f-32483c6d35f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8916385B-7771-4B86-AC30-95BD0DD5FA1F}">
   <ds:schemaRefs>

</xml_diff>